<commit_message>
Update Excels : Evaluation & Backlog
</commit_message>
<xml_diff>
--- a/Documents/0-Consignes/Evaluation Gr29.xlsx
+++ b/Documents/0-Consignes/Evaluation Gr29.xlsx
@@ -1,33 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10413"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Web2.0\Documents\0-Consignes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ephec-my.sharepoint.com/personal/he201742_students_ephec_be/Documents/0-COURS/BAC2/Q2/Dev_Info_Avance-Web/2-Projet/0-GitProjet_Gr29/Documents/0-Consignes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B5A0A98-7945-4064-A7CE-9E11ADD3BDA0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{3B5A0A98-7945-4064-A7CE-9E11ADD3BDA0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{8A8B41AB-FDA2-064C-A9BC-9467D1648AEF}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="16000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Grille" sheetId="1" r:id="rId1"/>
     <sheet name="Grille-résumé" sheetId="3" r:id="rId2"/>
     <sheet name="Rapport" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="240">
   <si>
     <t>La cote pour un projet qui respecte les critère de base est de 10/20.</t>
   </si>
@@ -731,9 +739,6 @@
     <t>Produit mais pas sur wiki</t>
   </si>
   <si>
-    <t>Completer avec le word de teams</t>
-  </si>
-  <si>
     <t>Wiki avec client</t>
   </si>
   <si>
@@ -741,6 +746,18 @@
   </si>
   <si>
     <t>CCL perso</t>
+  </si>
+  <si>
+    <t>Ajouter sur Wiki &amp; écrire retour de coaching restants</t>
+  </si>
+  <si>
+    <t>Completer si besoin + enlever "-" en trop</t>
+  </si>
+  <si>
+    <t>Faire Tests et compléter le Wiki</t>
+  </si>
+  <si>
+    <t>Implémenter le code</t>
   </si>
 </sst>
 </file>
@@ -1231,26 +1248,26 @@
       <selection activeCell="I122" sqref="I122"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="3" customWidth="1"/>
-    <col min="2" max="2" width="4.42578125" style="17" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="55.42578125" style="18" customWidth="1"/>
-    <col min="4" max="4" width="6.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.7109375" style="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.28515625" style="15" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="4.28515625" customWidth="1"/>
-    <col min="8" max="8" width="5.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="120.140625" style="18" customWidth="1"/>
-    <col min="10" max="10" width="46.85546875" customWidth="1"/>
+    <col min="2" max="2" width="4.5" style="17" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="55.5" style="18" customWidth="1"/>
+    <col min="4" max="4" width="6.83203125" style="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.6640625" style="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.33203125" style="15" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4.33203125" customWidth="1"/>
+    <col min="8" max="8" width="5.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="120.1640625" style="18" customWidth="1"/>
+    <col min="10" max="10" width="46.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:10" ht="16" x14ac:dyDescent="0.2">
       <c r="I1" s="18" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:10" ht="16" x14ac:dyDescent="0.2">
       <c r="E2" s="14">
         <v>10</v>
       </c>
@@ -1258,17 +1275,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:10" ht="16" x14ac:dyDescent="0.2">
       <c r="I3" s="18" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.2">
       <c r="D4" s="11"/>
       <c r="E4" s="13"/>
       <c r="F4" s="16"/>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.2">
       <c r="D5" s="11" t="s">
         <v>114</v>
       </c>
@@ -1279,7 +1296,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="6" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:10" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="B6" s="17"/>
       <c r="C6" s="19"/>
       <c r="D6" s="4" t="s">
@@ -1295,12 +1312,12 @@
         <v>201</v>
       </c>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.2">
       <c r="D7" s="11"/>
       <c r="E7" s="13"/>
       <c r="F7" s="16"/>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:10" ht="16" x14ac:dyDescent="0.2">
       <c r="B8" s="17" t="s">
         <v>147</v>
       </c>
@@ -1311,7 +1328,7 @@
       <c r="E8" s="13"/>
       <c r="F8" s="16"/>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:10" ht="16" x14ac:dyDescent="0.2">
       <c r="B9" s="17" t="s">
         <v>149</v>
       </c>
@@ -1340,7 +1357,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:10" ht="16" x14ac:dyDescent="0.2">
       <c r="D10" s="11"/>
       <c r="E10" s="13"/>
       <c r="F10" s="16"/>
@@ -1351,7 +1368,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:10" ht="16" x14ac:dyDescent="0.2">
       <c r="D11" s="11"/>
       <c r="E11" s="13"/>
       <c r="F11" s="16"/>
@@ -1362,12 +1379,12 @@
         <v>203</v>
       </c>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.2">
       <c r="D12" s="11"/>
       <c r="E12" s="13"/>
       <c r="F12" s="16"/>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:10" ht="16" x14ac:dyDescent="0.2">
       <c r="B13" s="17" t="s">
         <v>148</v>
       </c>
@@ -1396,7 +1413,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:10" ht="16" x14ac:dyDescent="0.2">
       <c r="D14" s="11"/>
       <c r="E14" s="13"/>
       <c r="F14" s="16"/>
@@ -1407,7 +1424,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:10" ht="16" x14ac:dyDescent="0.2">
       <c r="D15" s="11"/>
       <c r="E15" s="13"/>
       <c r="F15" s="16"/>
@@ -1418,12 +1435,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:10" x14ac:dyDescent="0.2">
       <c r="D16" s="11"/>
       <c r="E16" s="13"/>
       <c r="F16" s="16"/>
     </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:10" ht="16" x14ac:dyDescent="0.2">
       <c r="B17" s="17" t="s">
         <v>150</v>
       </c>
@@ -1452,7 +1469,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:10" ht="16" x14ac:dyDescent="0.2">
       <c r="D18" s="11"/>
       <c r="E18" s="13"/>
       <c r="F18" s="16"/>
@@ -1463,12 +1480,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:10" x14ac:dyDescent="0.2">
       <c r="D19" s="11"/>
       <c r="E19" s="13"/>
       <c r="F19" s="16"/>
     </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:10" ht="16" x14ac:dyDescent="0.2">
       <c r="B20" s="17" t="s">
         <v>151</v>
       </c>
@@ -1492,7 +1509,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:10" ht="16" x14ac:dyDescent="0.2">
       <c r="D21" s="11"/>
       <c r="E21" s="13"/>
       <c r="F21" s="16"/>
@@ -1503,13 +1520,13 @@
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:10" x14ac:dyDescent="0.2">
       <c r="D22" s="11"/>
       <c r="E22" s="13"/>
       <c r="F22" s="16"/>
       <c r="H22" s="9"/>
     </row>
-    <row r="23" spans="2:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:10" ht="32" x14ac:dyDescent="0.2">
       <c r="B23" s="17" t="s">
         <v>152</v>
       </c>
@@ -1538,7 +1555,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="24" spans="2:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:10" ht="32" x14ac:dyDescent="0.2">
       <c r="D24" s="11"/>
       <c r="E24" s="13"/>
       <c r="F24" s="16"/>
@@ -1547,7 +1564,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="25" spans="2:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:10" ht="32" x14ac:dyDescent="0.2">
       <c r="D25" s="11"/>
       <c r="E25" s="13"/>
       <c r="F25" s="16"/>
@@ -1556,12 +1573,12 @@
         <v>144</v>
       </c>
     </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:10" x14ac:dyDescent="0.2">
       <c r="D26" s="11"/>
       <c r="E26" s="13"/>
       <c r="F26" s="16"/>
     </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:10" ht="16" x14ac:dyDescent="0.2">
       <c r="B27" s="17" t="s">
         <v>153</v>
       </c>
@@ -1572,7 +1589,7 @@
       <c r="E27" s="13"/>
       <c r="F27" s="16"/>
     </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:10" ht="16" x14ac:dyDescent="0.2">
       <c r="B28" s="17" t="s">
         <v>154</v>
       </c>
@@ -1601,7 +1618,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="29" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:10" ht="16" x14ac:dyDescent="0.2">
       <c r="D29" s="11"/>
       <c r="E29" s="13"/>
       <c r="F29" s="16"/>
@@ -1612,12 +1629,12 @@
         <v>21</v>
       </c>
     </row>
-    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:10" x14ac:dyDescent="0.2">
       <c r="D30" s="11"/>
       <c r="E30" s="13"/>
       <c r="F30" s="16"/>
     </row>
-    <row r="31" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:10" ht="16" x14ac:dyDescent="0.2">
       <c r="B31" s="17" t="s">
         <v>155</v>
       </c>
@@ -1646,7 +1663,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="32" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:10" ht="16" x14ac:dyDescent="0.2">
       <c r="D32" s="11"/>
       <c r="E32" s="13"/>
       <c r="F32" s="16"/>
@@ -1657,7 +1674,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="33" spans="2:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:10" ht="32" x14ac:dyDescent="0.2">
       <c r="D33" s="11"/>
       <c r="E33" s="13"/>
       <c r="F33" s="16"/>
@@ -1668,12 +1685,12 @@
         <v>121</v>
       </c>
     </row>
-    <row r="34" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:10" x14ac:dyDescent="0.2">
       <c r="D34" s="11"/>
       <c r="E34" s="13"/>
       <c r="F34" s="16"/>
     </row>
-    <row r="35" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:10" ht="16" x14ac:dyDescent="0.2">
       <c r="B35" s="17" t="s">
         <v>156</v>
       </c>
@@ -1702,7 +1719,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="36" spans="2:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:10" ht="32" x14ac:dyDescent="0.2">
       <c r="D36" s="11"/>
       <c r="E36" s="13"/>
       <c r="F36" s="16"/>
@@ -1713,12 +1730,12 @@
         <v>122</v>
       </c>
     </row>
-    <row r="37" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:10" x14ac:dyDescent="0.2">
       <c r="D37" s="11"/>
       <c r="E37" s="13"/>
       <c r="F37" s="16"/>
     </row>
-    <row r="38" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:10" ht="16" x14ac:dyDescent="0.2">
       <c r="B38" s="17" t="s">
         <v>157</v>
       </c>
@@ -1744,7 +1761,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="39" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:10" ht="16" x14ac:dyDescent="0.2">
       <c r="D39" s="11"/>
       <c r="E39" s="13"/>
       <c r="F39" s="16"/>
@@ -1755,12 +1772,12 @@
         <v>28</v>
       </c>
     </row>
-    <row r="40" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:10" x14ac:dyDescent="0.2">
       <c r="D40" s="11"/>
       <c r="E40" s="13"/>
       <c r="F40" s="16"/>
     </row>
-    <row r="41" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:10" ht="16" x14ac:dyDescent="0.2">
       <c r="B41" s="17" t="s">
         <v>158</v>
       </c>
@@ -1771,7 +1788,7 @@
       <c r="E41" s="13"/>
       <c r="F41" s="16"/>
     </row>
-    <row r="42" spans="2:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:10" ht="48" x14ac:dyDescent="0.2">
       <c r="B42" s="17" t="s">
         <v>159</v>
       </c>
@@ -1798,7 +1815,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="43" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:10" ht="16" x14ac:dyDescent="0.2">
       <c r="D43" s="11"/>
       <c r="E43" s="13"/>
       <c r="F43" s="16"/>
@@ -1809,7 +1826,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="44" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:10" ht="16" x14ac:dyDescent="0.2">
       <c r="D44" s="11"/>
       <c r="E44" s="13"/>
       <c r="F44" s="16"/>
@@ -1820,12 +1837,12 @@
         <v>33</v>
       </c>
     </row>
-    <row r="45" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:10" x14ac:dyDescent="0.2">
       <c r="D45" s="11"/>
       <c r="E45" s="13"/>
       <c r="F45" s="16"/>
     </row>
-    <row r="46" spans="2:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:10" ht="16" x14ac:dyDescent="0.2">
       <c r="B46" s="17" t="s">
         <v>160</v>
       </c>
@@ -1851,7 +1868,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="47" spans="2:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:10" ht="32" x14ac:dyDescent="0.2">
       <c r="D47" s="11"/>
       <c r="E47" s="13"/>
       <c r="F47" s="16"/>
@@ -1862,7 +1879,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="48" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:10" ht="16" x14ac:dyDescent="0.2">
       <c r="D48" s="11"/>
       <c r="E48" s="13"/>
       <c r="F48" s="16"/>
@@ -1873,12 +1890,12 @@
         <v>36</v>
       </c>
     </row>
-    <row r="49" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:10" x14ac:dyDescent="0.2">
       <c r="D49" s="11"/>
       <c r="E49" s="13"/>
       <c r="F49" s="16"/>
     </row>
-    <row r="50" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:10" ht="16" x14ac:dyDescent="0.2">
       <c r="B50" s="17" t="s">
         <v>161</v>
       </c>
@@ -1907,7 +1924,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="51" spans="2:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:10" ht="32" x14ac:dyDescent="0.2">
       <c r="D51" s="11"/>
       <c r="E51" s="13"/>
       <c r="F51" s="16"/>
@@ -1918,12 +1935,12 @@
         <v>190</v>
       </c>
     </row>
-    <row r="52" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:10" x14ac:dyDescent="0.2">
       <c r="D52" s="11"/>
       <c r="E52" s="13"/>
       <c r="F52" s="16"/>
     </row>
-    <row r="53" spans="2:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:10" ht="48" x14ac:dyDescent="0.2">
       <c r="B53" s="17" t="s">
         <v>162</v>
       </c>
@@ -1952,17 +1969,17 @@
         <v>214</v>
       </c>
     </row>
-    <row r="54" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:10" x14ac:dyDescent="0.2">
       <c r="D54" s="11"/>
       <c r="E54" s="13"/>
       <c r="F54" s="16"/>
     </row>
-    <row r="55" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:10" x14ac:dyDescent="0.2">
       <c r="D55" s="11"/>
       <c r="E55" s="13"/>
       <c r="F55" s="16"/>
     </row>
-    <row r="56" spans="2:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:10" ht="16" x14ac:dyDescent="0.2">
       <c r="B56" s="17" t="s">
         <v>163</v>
       </c>
@@ -1988,18 +2005,18 @@
         <v>191</v>
       </c>
     </row>
-    <row r="57" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:10" x14ac:dyDescent="0.2">
       <c r="D57" s="11"/>
       <c r="E57" s="13"/>
       <c r="F57" s="16"/>
       <c r="H57" s="9"/>
     </row>
-    <row r="58" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:10" x14ac:dyDescent="0.2">
       <c r="D58" s="11"/>
       <c r="E58" s="13"/>
       <c r="F58" s="16"/>
     </row>
-    <row r="59" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:10" ht="16" x14ac:dyDescent="0.2">
       <c r="B59" s="17" t="s">
         <v>164</v>
       </c>
@@ -2010,7 +2027,7 @@
       <c r="E59" s="13"/>
       <c r="F59" s="16"/>
     </row>
-    <row r="60" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:10" ht="16" x14ac:dyDescent="0.2">
       <c r="B60" s="17" t="s">
         <v>165</v>
       </c>
@@ -2039,7 +2056,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="61" spans="2:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:10" ht="32" x14ac:dyDescent="0.2">
       <c r="D61" s="11"/>
       <c r="E61" s="13"/>
       <c r="F61" s="16"/>
@@ -2050,12 +2067,12 @@
         <v>44</v>
       </c>
     </row>
-    <row r="62" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:10" x14ac:dyDescent="0.2">
       <c r="D62" s="11"/>
       <c r="E62" s="13"/>
       <c r="F62" s="16"/>
     </row>
-    <row r="63" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:10" ht="16" x14ac:dyDescent="0.2">
       <c r="B63" s="17" t="s">
         <v>166</v>
       </c>
@@ -2084,7 +2101,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="64" spans="2:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:10" ht="16" x14ac:dyDescent="0.2">
       <c r="D64" s="11"/>
       <c r="E64" s="13"/>
       <c r="F64" s="16"/>
@@ -2095,12 +2112,12 @@
         <v>146</v>
       </c>
     </row>
-    <row r="65" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:10" x14ac:dyDescent="0.2">
       <c r="D65" s="11"/>
       <c r="E65" s="13"/>
       <c r="F65" s="16"/>
     </row>
-    <row r="66" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:10" ht="16" x14ac:dyDescent="0.2">
       <c r="B66" s="17" t="s">
         <v>167</v>
       </c>
@@ -2129,7 +2146,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="67" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:10" ht="16" x14ac:dyDescent="0.2">
       <c r="D67" s="11"/>
       <c r="E67" s="13"/>
       <c r="F67" s="16"/>
@@ -2140,12 +2157,12 @@
         <v>48</v>
       </c>
     </row>
-    <row r="68" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:10" x14ac:dyDescent="0.2">
       <c r="D68" s="11"/>
       <c r="E68" s="13"/>
       <c r="F68" s="16"/>
     </row>
-    <row r="69" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:10" ht="16" x14ac:dyDescent="0.2">
       <c r="B69" s="17" t="s">
         <v>168</v>
       </c>
@@ -2171,7 +2188,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="70" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:10" ht="16" x14ac:dyDescent="0.2">
       <c r="D70" s="11"/>
       <c r="E70" s="13"/>
       <c r="F70" s="16"/>
@@ -2182,12 +2199,12 @@
         <v>127</v>
       </c>
     </row>
-    <row r="71" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:10" x14ac:dyDescent="0.2">
       <c r="D71" s="11"/>
       <c r="E71" s="13"/>
       <c r="F71" s="16"/>
     </row>
-    <row r="72" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:10" ht="16" x14ac:dyDescent="0.2">
       <c r="B72" s="17" t="s">
         <v>169</v>
       </c>
@@ -2216,7 +2233,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="73" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:10" ht="16" x14ac:dyDescent="0.2">
       <c r="D73" s="11"/>
       <c r="E73" s="13"/>
       <c r="F73" s="16"/>
@@ -2227,12 +2244,12 @@
         <v>50</v>
       </c>
     </row>
-    <row r="74" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:10" x14ac:dyDescent="0.2">
       <c r="D74" s="11"/>
       <c r="E74" s="13"/>
       <c r="F74" s="16"/>
     </row>
-    <row r="75" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:10" ht="16" x14ac:dyDescent="0.2">
       <c r="B75" s="17" t="s">
         <v>170</v>
       </c>
@@ -2258,7 +2275,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="76" spans="2:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:10" ht="32" x14ac:dyDescent="0.2">
       <c r="D76" s="11"/>
       <c r="E76" s="13"/>
       <c r="F76" s="16"/>
@@ -2269,12 +2286,12 @@
         <v>53</v>
       </c>
     </row>
-    <row r="77" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:10" x14ac:dyDescent="0.2">
       <c r="D77" s="11"/>
       <c r="E77" s="13"/>
       <c r="F77" s="16"/>
     </row>
-    <row r="78" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:10" ht="16" x14ac:dyDescent="0.2">
       <c r="B78" s="17" t="s">
         <v>171</v>
       </c>
@@ -2300,7 +2317,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="79" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:10" ht="16" x14ac:dyDescent="0.2">
       <c r="D79" s="11"/>
       <c r="E79" s="13"/>
       <c r="F79" s="16"/>
@@ -2311,12 +2328,12 @@
         <v>113</v>
       </c>
     </row>
-    <row r="80" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:10" x14ac:dyDescent="0.2">
       <c r="D80" s="11"/>
       <c r="E80" s="13"/>
       <c r="F80" s="16"/>
     </row>
-    <row r="81" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:10" ht="16" x14ac:dyDescent="0.2">
       <c r="B81" s="17" t="s">
         <v>172</v>
       </c>
@@ -2343,7 +2360,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="82" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:10" ht="16" x14ac:dyDescent="0.2">
       <c r="D82" s="11"/>
       <c r="E82" s="13"/>
       <c r="F82" s="16"/>
@@ -2354,7 +2371,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="83" spans="2:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:10" ht="32" x14ac:dyDescent="0.2">
       <c r="D83" s="11"/>
       <c r="E83" s="13"/>
       <c r="F83" s="16"/>
@@ -2365,12 +2382,12 @@
         <v>202</v>
       </c>
     </row>
-    <row r="84" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:10" x14ac:dyDescent="0.2">
       <c r="D84" s="11"/>
       <c r="E84" s="13"/>
       <c r="F84" s="16"/>
     </row>
-    <row r="85" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:10" ht="16" x14ac:dyDescent="0.2">
       <c r="B85" s="17" t="s">
         <v>173</v>
       </c>
@@ -2381,7 +2398,7 @@
       <c r="E85" s="13"/>
       <c r="F85" s="16"/>
     </row>
-    <row r="86" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:10" ht="16" x14ac:dyDescent="0.2">
       <c r="B86" s="17" t="s">
         <v>174</v>
       </c>
@@ -2410,7 +2427,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="87" spans="2:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:10" ht="32" x14ac:dyDescent="0.2">
       <c r="D87" s="11"/>
       <c r="E87" s="13"/>
       <c r="F87" s="16"/>
@@ -2421,12 +2438,12 @@
         <v>44</v>
       </c>
     </row>
-    <row r="88" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:10" x14ac:dyDescent="0.2">
       <c r="D88" s="11"/>
       <c r="E88" s="13"/>
       <c r="F88" s="16"/>
     </row>
-    <row r="89" spans="2:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:10" ht="16" x14ac:dyDescent="0.2">
       <c r="B89" s="17" t="s">
         <v>175</v>
       </c>
@@ -2455,7 +2472,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="90" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:10" ht="16" x14ac:dyDescent="0.2">
       <c r="D90" s="11"/>
       <c r="E90" s="13"/>
       <c r="F90" s="16"/>
@@ -2466,12 +2483,12 @@
         <v>61</v>
       </c>
     </row>
-    <row r="91" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:10" x14ac:dyDescent="0.2">
       <c r="D91" s="11"/>
       <c r="E91" s="13"/>
       <c r="F91" s="16"/>
     </row>
-    <row r="92" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:10" ht="16" x14ac:dyDescent="0.2">
       <c r="B92" s="17" t="s">
         <v>176</v>
       </c>
@@ -2500,7 +2517,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="93" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:10" ht="16" x14ac:dyDescent="0.2">
       <c r="D93" s="11"/>
       <c r="E93" s="13"/>
       <c r="F93" s="16"/>
@@ -2511,12 +2528,12 @@
         <v>64</v>
       </c>
     </row>
-    <row r="94" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:10" x14ac:dyDescent="0.2">
       <c r="D94" s="11"/>
       <c r="E94" s="13"/>
       <c r="F94" s="16"/>
     </row>
-    <row r="95" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="95" spans="2:10" ht="16" x14ac:dyDescent="0.2">
       <c r="B95" s="17" t="s">
         <v>177</v>
       </c>
@@ -2545,7 +2562,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="96" spans="2:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="96" spans="2:10" ht="16" x14ac:dyDescent="0.2">
       <c r="D96" s="11"/>
       <c r="E96" s="13"/>
       <c r="F96" s="16"/>
@@ -2556,7 +2573,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="97" spans="2:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:9" ht="32" x14ac:dyDescent="0.2">
       <c r="D97" s="11"/>
       <c r="E97" s="13"/>
       <c r="F97" s="16"/>
@@ -2567,12 +2584,12 @@
         <v>129</v>
       </c>
     </row>
-    <row r="98" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="98" spans="2:9" x14ac:dyDescent="0.2">
       <c r="D98" s="11"/>
       <c r="E98" s="13"/>
       <c r="F98" s="16"/>
     </row>
-    <row r="99" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="99" spans="2:9" ht="16" x14ac:dyDescent="0.2">
       <c r="B99" s="17" t="s">
         <v>178</v>
       </c>
@@ -2598,7 +2615,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="100" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="100" spans="2:9" ht="16" x14ac:dyDescent="0.2">
       <c r="D100" s="11"/>
       <c r="E100" s="13"/>
       <c r="F100" s="16"/>
@@ -2609,12 +2626,12 @@
         <v>128</v>
       </c>
     </row>
-    <row r="101" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="101" spans="2:9" x14ac:dyDescent="0.2">
       <c r="D101" s="11"/>
       <c r="E101" s="13"/>
       <c r="F101" s="16"/>
     </row>
-    <row r="102" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="102" spans="2:9" ht="16" x14ac:dyDescent="0.2">
       <c r="B102" s="17" t="s">
         <v>179</v>
       </c>
@@ -2625,7 +2642,7 @@
       <c r="E102" s="13"/>
       <c r="F102" s="16"/>
     </row>
-    <row r="103" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="103" spans="2:9" ht="16" x14ac:dyDescent="0.2">
       <c r="B103" s="17" t="s">
         <v>180</v>
       </c>
@@ -2649,7 +2666,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="104" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="104" spans="2:9" ht="16" x14ac:dyDescent="0.2">
       <c r="D104" s="11"/>
       <c r="E104" s="13"/>
       <c r="F104" s="16"/>
@@ -2660,7 +2677,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="105" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="105" spans="2:9" ht="16" x14ac:dyDescent="0.2">
       <c r="D105" s="11"/>
       <c r="E105" s="13"/>
       <c r="F105" s="16"/>
@@ -2671,12 +2688,12 @@
         <v>71</v>
       </c>
     </row>
-    <row r="106" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="106" spans="2:9" x14ac:dyDescent="0.2">
       <c r="D106" s="11"/>
       <c r="E106" s="13"/>
       <c r="F106" s="16"/>
     </row>
-    <row r="107" spans="2:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="107" spans="2:9" ht="16" x14ac:dyDescent="0.2">
       <c r="B107" s="17" t="s">
         <v>181</v>
       </c>
@@ -2700,12 +2717,12 @@
         <v>109</v>
       </c>
     </row>
-    <row r="108" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="108" spans="2:9" x14ac:dyDescent="0.2">
       <c r="D108" s="11"/>
       <c r="E108" s="13"/>
       <c r="F108" s="16"/>
     </row>
-    <row r="109" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="109" spans="2:9" ht="16" x14ac:dyDescent="0.2">
       <c r="B109" s="17" t="s">
         <v>182</v>
       </c>
@@ -2728,19 +2745,19 @@
         <v>74</v>
       </c>
     </row>
-    <row r="110" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="110" spans="2:9" x14ac:dyDescent="0.2">
       <c r="D110" s="11"/>
       <c r="E110" s="13"/>
       <c r="F110" s="16"/>
       <c r="H110" s="9"/>
     </row>
-    <row r="111" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="111" spans="2:9" x14ac:dyDescent="0.2">
       <c r="D111" s="11"/>
       <c r="E111" s="13"/>
       <c r="F111" s="16"/>
       <c r="H111" s="9"/>
     </row>
-    <row r="112" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="112" spans="2:9" ht="16" x14ac:dyDescent="0.2">
       <c r="B112" s="17">
         <v>7</v>
       </c>
@@ -2751,7 +2768,7 @@
       <c r="E112" s="13"/>
       <c r="F112" s="16"/>
     </row>
-    <row r="113" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="113" spans="2:9" ht="16" x14ac:dyDescent="0.2">
       <c r="B113" s="17" t="s">
         <v>183</v>
       </c>
@@ -2775,7 +2792,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="114" spans="2:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="114" spans="2:9" ht="32" x14ac:dyDescent="0.2">
       <c r="D114" s="11"/>
       <c r="E114" s="13"/>
       <c r="F114" s="16"/>
@@ -2786,12 +2803,12 @@
         <v>140</v>
       </c>
     </row>
-    <row r="115" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="115" spans="2:9" x14ac:dyDescent="0.2">
       <c r="D115" s="11"/>
       <c r="E115" s="13"/>
       <c r="F115" s="16"/>
     </row>
-    <row r="116" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="116" spans="2:9" ht="16" x14ac:dyDescent="0.2">
       <c r="B116" s="17" t="s">
         <v>184</v>
       </c>
@@ -2815,7 +2832,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="117" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="117" spans="2:9" ht="16" x14ac:dyDescent="0.2">
       <c r="D117" s="11"/>
       <c r="E117" s="13"/>
       <c r="F117" s="16"/>
@@ -2826,12 +2843,12 @@
         <v>141</v>
       </c>
     </row>
-    <row r="118" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="118" spans="2:9" x14ac:dyDescent="0.2">
       <c r="D118" s="11"/>
       <c r="E118" s="13"/>
       <c r="F118" s="16"/>
     </row>
-    <row r="119" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="119" spans="2:9" ht="16" x14ac:dyDescent="0.2">
       <c r="B119" s="17" t="s">
         <v>185</v>
       </c>
@@ -2855,7 +2872,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="120" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="120" spans="2:9" ht="16" x14ac:dyDescent="0.2">
       <c r="D120" s="11"/>
       <c r="E120" s="13"/>
       <c r="F120" s="16"/>
@@ -2866,23 +2883,23 @@
         <v>139</v>
       </c>
     </row>
-    <row r="121" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="121" spans="2:9" x14ac:dyDescent="0.2">
       <c r="D121" s="11"/>
       <c r="E121" s="13"/>
       <c r="F121" s="16"/>
     </row>
-    <row r="122" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="122" spans="2:9" x14ac:dyDescent="0.2">
       <c r="D122" s="11"/>
       <c r="E122" s="13"/>
       <c r="F122" s="16"/>
     </row>
-    <row r="124" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="124" spans="2:9" ht="16" x14ac:dyDescent="0.2">
       <c r="C124" s="28"/>
     </row>
-    <row r="125" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="125" spans="2:9" ht="16" x14ac:dyDescent="0.2">
       <c r="C125" s="28"/>
     </row>
-    <row r="126" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="126" spans="2:9" ht="16" x14ac:dyDescent="0.2">
       <c r="C126" s="29"/>
     </row>
   </sheetData>
@@ -2899,13 +2916,13 @@
       <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" style="2"/>
-    <col min="2" max="2" width="69.7109375" customWidth="1"/>
+    <col min="1" max="1" width="11.5" style="2"/>
+    <col min="2" max="2" width="69.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -2913,7 +2930,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>149</v>
       </c>
@@ -2921,7 +2938,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>148</v>
       </c>
@@ -2929,7 +2946,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>150</v>
       </c>
@@ -2937,7 +2954,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>151</v>
       </c>
@@ -2945,7 +2962,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>152</v>
       </c>
@@ -2953,7 +2970,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>2</v>
       </c>
@@ -2961,7 +2978,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>154</v>
       </c>
@@ -2969,7 +2986,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>155</v>
       </c>
@@ -2977,7 +2994,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>156</v>
       </c>
@@ -2985,7 +3002,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>157</v>
       </c>
@@ -2993,7 +3010,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>3</v>
       </c>
@@ -3001,7 +3018,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>159</v>
       </c>
@@ -3009,7 +3026,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>160</v>
       </c>
@@ -3017,7 +3034,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>161</v>
       </c>
@@ -3025,7 +3042,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>162</v>
       </c>
@@ -3033,7 +3050,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>163</v>
       </c>
@@ -3041,7 +3058,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>4</v>
       </c>
@@ -3049,7 +3066,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>165</v>
       </c>
@@ -3057,7 +3074,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>166</v>
       </c>
@@ -3065,7 +3082,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>167</v>
       </c>
@@ -3073,7 +3090,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>168</v>
       </c>
@@ -3081,7 +3098,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>169</v>
       </c>
@@ -3089,7 +3106,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>170</v>
       </c>
@@ -3097,7 +3114,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>171</v>
       </c>
@@ -3105,7 +3122,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>172</v>
       </c>
@@ -3113,7 +3130,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" s="2">
         <v>5</v>
       </c>
@@ -3121,7 +3138,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>174</v>
       </c>
@@ -3129,7 +3146,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>175</v>
       </c>
@@ -3137,7 +3154,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
         <v>176</v>
       </c>
@@ -3145,7 +3162,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
         <v>177</v>
       </c>
@@ -3153,7 +3170,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
         <v>178</v>
       </c>
@@ -3161,7 +3178,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" s="2">
         <v>6</v>
       </c>
@@ -3169,7 +3186,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
         <v>180</v>
       </c>
@@ -3177,7 +3194,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
         <v>181</v>
       </c>
@@ -3185,7 +3202,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
         <v>182</v>
       </c>
@@ -3193,7 +3210,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" s="2">
         <v>7</v>
       </c>
@@ -3201,7 +3218,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
         <v>183</v>
       </c>
@@ -3209,7 +3226,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
         <v>184</v>
       </c>
@@ -3217,7 +3234,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
         <v>185</v>
       </c>
@@ -3234,37 +3251,37 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A2:D27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="138.5703125" style="18" customWidth="1"/>
-    <col min="4" max="4" width="45.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="138.5" style="18" customWidth="1"/>
+    <col min="4" max="4" width="45.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B2" s="18" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B3" s="18" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B4" s="31" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B7" s="27" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>86</v>
       </c>
@@ -3272,10 +3289,10 @@
         <v>77</v>
       </c>
       <c r="C8" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>87</v>
       </c>
@@ -3283,10 +3300,10 @@
         <v>78</v>
       </c>
       <c r="C9" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>88</v>
       </c>
@@ -3297,7 +3314,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>89</v>
       </c>
@@ -3308,7 +3325,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>90</v>
       </c>
@@ -3319,7 +3336,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>91</v>
       </c>
@@ -3333,7 +3350,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>92</v>
       </c>
@@ -3344,7 +3361,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>93</v>
       </c>
@@ -3358,7 +3375,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>94</v>
       </c>
@@ -3369,7 +3386,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>95</v>
       </c>
@@ -3383,7 +3400,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>96</v>
       </c>
@@ -3397,7 +3414,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>97</v>
       </c>
@@ -3407,8 +3424,11 @@
       <c r="C19" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D19" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>98</v>
       </c>
@@ -3418,8 +3438,11 @@
       <c r="C20" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D20" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>99</v>
       </c>
@@ -3429,8 +3452,11 @@
       <c r="C21" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="D21" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>100</v>
       </c>
@@ -3441,7 +3467,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>101</v>
       </c>
@@ -3449,13 +3475,13 @@
         <v>194</v>
       </c>
       <c r="C23" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="D23" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>102</v>
       </c>
@@ -3466,10 +3492,10 @@
         <v>227</v>
       </c>
       <c r="D24" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>103</v>
       </c>
@@ -3480,10 +3506,10 @@
         <v>227</v>
       </c>
       <c r="D25" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>104</v>
       </c>
@@ -3494,10 +3520,10 @@
         <v>227</v>
       </c>
       <c r="D26" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="2"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
remarque ajouté grille de cotation
</commit_message>
<xml_diff>
--- a/Documents/0-Consignes/Evaluation Gr29.xlsx
+++ b/Documents/0-Consignes/Evaluation Gr29.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10510"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ephec-my.sharepoint.com/personal/he201742_students_ephec_be/Documents/0-COURS/BAC2/Q2/Dev_Info_Avance-Web/2-Projet/0-GitProjet_Gr29/Documents/0-Consignes/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Unif\OneDrive\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="114_{E2B6B17E-4704-1444-9082-F445CB12EE68}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88964288-B6BD-4802-94FD-5E15517829E9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="16480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Grille" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="262">
   <si>
     <t>min</t>
   </si>
@@ -753,6 +753,86 @@
     <t>Installation
 Faire un workflow des branches git et pq
 Sécurité</t>
+  </si>
+  <si>
+    <t>Notes groupes</t>
+  </si>
+  <si>
+    <t>Notes prof</t>
+  </si>
+  <si>
+    <t>Voulait clicable au lieu de bouton</t>
+  </si>
+  <si>
+    <t>En cas de DB down, pas de site</t>
+  </si>
+  <si>
+    <t>hyper résumé</t>
+  </si>
+  <si>
+    <t>ok dans excel donc bonus</t>
+  </si>
+  <si>
+    <t>page dans titre, api dans task</t>
+  </si>
+  <si>
+    <t>res.render sur le résultat, traite pas l'erreur</t>
+  </si>
+  <si>
+    <t>prof va vérifier</t>
+  </si>
+  <si>
+    <t>branches par features
+gael moins de commit du a sa manière de travailler
+fin de certaines branches encore a merger</t>
+  </si>
+  <si>
+    <t>dans excel
+résumé dans wiki</t>
+  </si>
+  <si>
+    <t>non</t>
+  </si>
+  <si>
+    <t xml:space="preserve">node.js bien : js // express à découvrir
+node à part ressemble pas à js … impresion de faire du java … // pas clair
+SUPER ABSTRAIT // pour token require // communiquer backend front end se renseigner et ont mis en place des …tableaux // entre différentes pages on s'envoient des données… </t>
+  </si>
+  <si>
+    <t>base générée en webstorm</t>
+  </si>
+  <si>
+    <t>pas été tres en détails, semblent bien connaitre</t>
+  </si>
+  <si>
+    <t>OK dans wiki directement</t>
+  </si>
+  <si>
+    <t>format de réponse serait mieux du json directement</t>
+  </si>
+  <si>
+    <t>manque login pas encore complet</t>
+  </si>
+  <si>
+    <t>postman</t>
+  </si>
+  <si>
+    <t>mysql ? Pq pas mariadb?</t>
+  </si>
+  <si>
+    <t>Opensource pas clair</t>
+  </si>
+  <si>
+    <t>comprennent leur connexion mais bof</t>
+  </si>
+  <si>
+    <t>diagramme ER ok</t>
+  </si>
+  <si>
+    <t>pas encore en ligne</t>
+  </si>
+  <si>
+    <t>Attention en root et sans password</t>
   </si>
 </sst>
 </file>
@@ -1137,7 +1217,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="119">
+  <cellXfs count="121">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1472,6 +1552,10 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1774,26 +1858,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I93"/>
+  <dimension ref="A1:J93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F33" sqref="F33:F35"/>
+    <sheetView tabSelected="1" topLeftCell="A74" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J88" sqref="J88"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.5" style="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.83203125" style="16" customWidth="1"/>
-    <col min="3" max="3" width="6.33203125" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.5" style="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.5" style="13" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.33203125" customWidth="1"/>
-    <col min="7" max="7" width="5.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="77.83203125" style="16" customWidth="1"/>
-    <col min="9" max="9" width="63.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.42578125" style="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.85546875" style="16" customWidth="1"/>
+    <col min="3" max="3" width="6.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.42578125" style="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.28515625" customWidth="1"/>
+    <col min="7" max="7" width="5.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="77.85546875" style="16" customWidth="1"/>
+    <col min="9" max="9" width="63.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="49.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C1" s="9" t="s">
         <v>112</v>
       </c>
@@ -1804,7 +1889,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="15"/>
       <c r="B2" s="17"/>
       <c r="C2" s="4" t="s">
@@ -1819,8 +1904,14 @@
       <c r="H2" s="17" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I2" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="22" t="s">
         <v>143</v>
       </c>
@@ -1831,7 +1922,7 @@
       <c r="D3" s="11"/>
       <c r="E3" s="14"/>
     </row>
-    <row r="4" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="102" t="s">
         <v>145</v>
       </c>
@@ -1858,7 +1949,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="98"/>
       <c r="B5" s="97"/>
       <c r="C5" s="111"/>
@@ -1872,7 +1963,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="98"/>
       <c r="B6" s="97"/>
       <c r="C6" s="111"/>
@@ -1886,7 +1977,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="98" t="s">
         <v>144</v>
       </c>
@@ -1912,8 +2003,11 @@
       <c r="I7" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="J7" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="98"/>
       <c r="B8" s="97"/>
       <c r="C8" s="111"/>
@@ -1927,7 +2021,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="98"/>
       <c r="B9" s="97"/>
       <c r="C9" s="111"/>
@@ -1941,7 +2035,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="98" t="s">
         <v>146</v>
       </c>
@@ -1968,7 +2062,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="98"/>
       <c r="B11" s="97"/>
       <c r="C11" s="111"/>
@@ -1982,7 +2076,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="96" t="s">
         <v>147</v>
       </c>
@@ -2005,8 +2099,11 @@
       <c r="H12" s="38" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="J12" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="96"/>
       <c r="B13" s="97"/>
       <c r="C13" s="111"/>
@@ -2020,7 +2117,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="103" t="s">
         <v>148</v>
       </c>
@@ -2044,7 +2141,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="103"/>
       <c r="B15" s="97"/>
       <c r="C15" s="111"/>
@@ -2056,7 +2153,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="33" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="104"/>
       <c r="B16" s="105"/>
       <c r="C16" s="112"/>
@@ -2068,7 +2165,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="24"/>
       <c r="B17" s="23"/>
       <c r="C17" s="25"/>
@@ -2076,7 +2173,7 @@
       <c r="E17" s="29"/>
       <c r="F17" s="65"/>
     </row>
-    <row r="18" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="52" t="s">
         <v>149</v>
       </c>
@@ -2088,7 +2185,7 @@
       <c r="E18" s="30"/>
       <c r="F18" s="65"/>
     </row>
-    <row r="19" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="102" t="s">
         <v>150</v>
       </c>
@@ -2116,8 +2213,11 @@
       <c r="I19" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="J19" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="98"/>
       <c r="B20" s="97"/>
       <c r="C20" s="111"/>
@@ -2131,7 +2231,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="98" t="s">
         <v>151</v>
       </c>
@@ -2159,8 +2259,11 @@
       <c r="I21" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="J21" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="98"/>
       <c r="B22" s="97"/>
       <c r="C22" s="111"/>
@@ -2174,7 +2277,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" s="98"/>
       <c r="B23" s="97"/>
       <c r="C23" s="111"/>
@@ -2188,7 +2291,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="98" t="s">
         <v>152</v>
       </c>
@@ -2216,8 +2319,11 @@
       <c r="I24" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+      <c r="J24" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" s="98"/>
       <c r="B25" s="97"/>
       <c r="C25" s="111"/>
@@ -2234,7 +2340,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="98" t="s">
         <v>153</v>
       </c>
@@ -2259,8 +2365,11 @@
       <c r="H26" s="38" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="27" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="J26" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="108"/>
       <c r="B27" s="105"/>
       <c r="C27" s="112"/>
@@ -2274,7 +2383,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="24"/>
       <c r="B28" s="23"/>
       <c r="C28" s="25"/>
@@ -2282,7 +2391,7 @@
       <c r="E28" s="29"/>
       <c r="F28" s="65"/>
     </row>
-    <row r="29" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="52" t="s">
         <v>154</v>
       </c>
@@ -2294,7 +2403,7 @@
       <c r="E29" s="30"/>
       <c r="F29" s="65"/>
     </row>
-    <row r="30" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A30" s="107" t="s">
         <v>155</v>
       </c>
@@ -2320,8 +2429,11 @@
       <c r="I30" s="16" t="s">
         <v>236</v>
       </c>
-    </row>
-    <row r="31" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="J30" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="96"/>
       <c r="B31" s="97"/>
       <c r="C31" s="111"/>
@@ -2335,7 +2447,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="96"/>
       <c r="B32" s="97"/>
       <c r="C32" s="111"/>
@@ -2349,7 +2461,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A33" s="98" t="s">
         <v>156</v>
       </c>
@@ -2374,8 +2486,11 @@
       <c r="H33" s="38" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="34" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+      <c r="J33" s="16" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A34" s="98"/>
       <c r="B34" s="97"/>
       <c r="C34" s="111"/>
@@ -2389,7 +2504,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="98"/>
       <c r="B35" s="97"/>
       <c r="C35" s="111"/>
@@ -2403,7 +2518,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="98" t="s">
         <v>157</v>
       </c>
@@ -2432,7 +2547,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="37" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A37" s="98"/>
       <c r="B37" s="97"/>
       <c r="C37" s="111"/>
@@ -2446,7 +2561,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="38" spans="1:9" ht="64" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A38" s="62" t="s">
         <v>158</v>
       </c>
@@ -2474,8 +2589,11 @@
       <c r="I38" s="16" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="39" spans="1:9" ht="33" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="J38" s="16" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="55" t="s">
         <v>159</v>
       </c>
@@ -2500,8 +2618,11 @@
       <c r="H39" s="40" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J39" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="24"/>
       <c r="B40" s="23"/>
       <c r="C40" s="25"/>
@@ -2510,7 +2631,7 @@
       <c r="F40" s="65"/>
       <c r="G40" s="7"/>
     </row>
-    <row r="41" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="52" t="s">
         <v>160</v>
       </c>
@@ -2522,7 +2643,7 @@
       <c r="E41" s="30"/>
       <c r="F41" s="65"/>
     </row>
-    <row r="42" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:10" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="99" t="s">
         <v>161</v>
       </c>
@@ -2550,8 +2671,11 @@
       <c r="I42" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="43" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+      <c r="J42" s="120" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A43" s="100"/>
       <c r="B43" s="97"/>
       <c r="C43" s="111"/>
@@ -2564,8 +2688,9 @@
       <c r="H43" s="38" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="44" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="J43" s="120"/>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="96" t="s">
         <v>162</v>
       </c>
@@ -2593,8 +2718,11 @@
       <c r="I44" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="45" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+      <c r="J44" s="119" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="96"/>
       <c r="B45" s="97"/>
       <c r="C45" s="111"/>
@@ -2610,8 +2738,11 @@
       <c r="I45" s="56" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="46" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="J45" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="98" t="s">
         <v>163</v>
       </c>
@@ -2636,8 +2767,11 @@
       <c r="H46" s="38" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="47" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+      <c r="J46" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" s="98"/>
       <c r="B47" s="97"/>
       <c r="C47" s="111"/>
@@ -2650,8 +2784,11 @@
       <c r="H47" s="38" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J47" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="98" t="s">
         <v>164</v>
       </c>
@@ -2677,8 +2814,11 @@
       <c r="I48" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="49" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+      <c r="J48" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="98"/>
       <c r="B49" s="97"/>
       <c r="C49" s="111"/>
@@ -2695,7 +2835,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="50" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A50" s="96" t="s">
         <v>165</v>
       </c>
@@ -2723,8 +2863,11 @@
       <c r="I50" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="51" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+      <c r="J50" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="96"/>
       <c r="B51" s="97"/>
       <c r="C51" s="111"/>
@@ -2738,7 +2881,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="52" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="98" t="s">
         <v>166</v>
       </c>
@@ -2763,8 +2906,11 @@
       <c r="H52" s="38" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="53" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+      <c r="J52" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A53" s="98"/>
       <c r="B53" s="97"/>
       <c r="C53" s="111"/>
@@ -2777,8 +2923,11 @@
       <c r="H53" s="38" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="54" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="J53" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A54" s="98" t="s">
         <v>167</v>
       </c>
@@ -2803,8 +2952,11 @@
       <c r="H54" s="38" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="55" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="J54" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="98"/>
       <c r="B55" s="97"/>
       <c r="C55" s="111"/>
@@ -2817,8 +2969,11 @@
       <c r="H55" s="38" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="56" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="J55" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="103" t="s">
         <v>168</v>
       </c>
@@ -2844,8 +2999,11 @@
       <c r="I56" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="57" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+      <c r="J56" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A57" s="103"/>
       <c r="B57" s="97"/>
       <c r="C57" s="111"/>
@@ -2859,7 +3017,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="58" spans="1:9" ht="33" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="104"/>
       <c r="B58" s="105"/>
       <c r="C58" s="112"/>
@@ -2873,7 +3031,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" s="24"/>
       <c r="B59" s="23"/>
       <c r="C59" s="25"/>
@@ -2881,7 +3039,7 @@
       <c r="E59" s="29"/>
       <c r="F59" s="65"/>
     </row>
-    <row r="60" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="52" t="s">
         <v>169</v>
       </c>
@@ -2893,7 +3051,7 @@
       <c r="E60" s="30"/>
       <c r="F60" s="65"/>
     </row>
-    <row r="61" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" s="102" t="s">
         <v>170</v>
       </c>
@@ -2920,7 +3078,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="62" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A62" s="98"/>
       <c r="B62" s="97"/>
       <c r="C62" s="111"/>
@@ -2934,7 +3092,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="63" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" s="98" t="s">
         <v>171</v>
       </c>
@@ -2961,7 +3119,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="64" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" s="98"/>
       <c r="B64" s="97"/>
       <c r="C64" s="111"/>
@@ -2975,7 +3133,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="65" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" s="96" t="s">
         <v>172</v>
       </c>
@@ -3002,7 +3160,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="66" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" s="96"/>
       <c r="B66" s="97"/>
       <c r="C66" s="111"/>
@@ -3016,7 +3174,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="67" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" s="96" t="s">
         <v>173</v>
       </c>
@@ -3043,7 +3201,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="68" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A68" s="96"/>
       <c r="B68" s="97"/>
       <c r="C68" s="111"/>
@@ -3057,7 +3215,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="69" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A69" s="96"/>
       <c r="B69" s="97"/>
       <c r="C69" s="111"/>
@@ -3071,7 +3229,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="70" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" s="98" t="s">
         <v>174</v>
       </c>
@@ -3095,7 +3253,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="71" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A71" s="108"/>
       <c r="B71" s="105"/>
       <c r="C71" s="112"/>
@@ -3109,7 +3267,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" s="24"/>
       <c r="B72" s="23"/>
       <c r="C72" s="25"/>
@@ -3117,7 +3275,7 @@
       <c r="E72" s="29"/>
       <c r="F72" s="65"/>
     </row>
-    <row r="73" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A73" s="52" t="s">
         <v>175</v>
       </c>
@@ -3129,7 +3287,7 @@
       <c r="E73" s="30"/>
       <c r="F73" s="65"/>
     </row>
-    <row r="74" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" s="109" t="s">
         <v>176</v>
       </c>
@@ -3156,7 +3314,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="75" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A75" s="103"/>
       <c r="B75" s="97"/>
       <c r="C75" s="111"/>
@@ -3170,7 +3328,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="76" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" s="103"/>
       <c r="B76" s="97"/>
       <c r="C76" s="111"/>
@@ -3184,7 +3342,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="77" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A77" s="54" t="s">
         <v>177</v>
       </c>
@@ -3208,7 +3366,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="78" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A78" s="55" t="s">
         <v>178</v>
       </c>
@@ -3232,7 +3390,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" s="24"/>
       <c r="B79" s="23"/>
       <c r="C79" s="25"/>
@@ -3241,7 +3399,7 @@
       <c r="F79" s="65"/>
       <c r="G79" s="7"/>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80" s="24"/>
       <c r="B80" s="23"/>
       <c r="C80" s="25"/>
@@ -3250,7 +3408,7 @@
       <c r="F80" s="65"/>
       <c r="G80" s="7"/>
     </row>
-    <row r="81" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A81" s="52">
         <v>7</v>
       </c>
@@ -3262,7 +3420,7 @@
       <c r="E81" s="30"/>
       <c r="F81" s="65"/>
     </row>
-    <row r="82" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" s="107" t="s">
         <v>179</v>
       </c>
@@ -3286,7 +3444,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="83" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A83" s="96"/>
       <c r="B83" s="97"/>
       <c r="C83" s="111"/>
@@ -3303,7 +3461,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="84" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" s="96" t="s">
         <v>180</v>
       </c>
@@ -3328,7 +3486,7 @@
       </c>
       <c r="I84" s="56"/>
     </row>
-    <row r="85" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A85" s="96"/>
       <c r="B85" s="97"/>
       <c r="C85" s="111"/>
@@ -3345,7 +3503,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="86" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86" s="96" t="s">
         <v>181</v>
       </c>
@@ -3370,7 +3528,7 @@
       </c>
       <c r="I86" s="56"/>
     </row>
-    <row r="87" spans="1:9" ht="33" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A87" s="106"/>
       <c r="B87" s="105"/>
       <c r="C87" s="112"/>
@@ -3386,33 +3544,37 @@
       <c r="I87" s="56" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J87" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C88" s="9"/>
       <c r="D88" s="11"/>
       <c r="E88" s="14"/>
       <c r="I88" s="56"/>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C89" s="9"/>
       <c r="D89" s="11"/>
       <c r="E89" s="14"/>
       <c r="I89" s="56"/>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="I90" s="56"/>
     </row>
-    <row r="91" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B91" s="18"/>
     </row>
-    <row r="92" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B92" s="18"/>
     </row>
-    <row r="93" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B93" s="19"/>
     </row>
   </sheetData>
-  <mergeCells count="174">
+  <mergeCells count="175">
+    <mergeCell ref="J42:J43"/>
     <mergeCell ref="C86:C87"/>
     <mergeCell ref="D86:D87"/>
     <mergeCell ref="E86:E87"/>
@@ -3608,13 +3770,13 @@
       <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.5" style="2"/>
-    <col min="2" max="2" width="69.6640625" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" style="2"/>
+    <col min="2" max="2" width="69.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -3622,7 +3784,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>145</v>
       </c>
@@ -3630,7 +3792,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>144</v>
       </c>
@@ -3638,7 +3800,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>146</v>
       </c>
@@ -3646,7 +3808,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>147</v>
       </c>
@@ -3654,7 +3816,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>148</v>
       </c>
@@ -3662,7 +3824,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>2</v>
       </c>
@@ -3670,7 +3832,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>150</v>
       </c>
@@ -3678,7 +3840,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>151</v>
       </c>
@@ -3686,7 +3848,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>152</v>
       </c>
@@ -3694,7 +3856,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>153</v>
       </c>
@@ -3702,7 +3864,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>3</v>
       </c>
@@ -3710,7 +3872,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>155</v>
       </c>
@@ -3718,7 +3880,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>156</v>
       </c>
@@ -3726,7 +3888,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>157</v>
       </c>
@@ -3734,7 +3896,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>158</v>
       </c>
@@ -3742,7 +3904,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>159</v>
       </c>
@@ -3750,7 +3912,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>4</v>
       </c>
@@ -3758,7 +3920,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>161</v>
       </c>
@@ -3766,7 +3928,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>162</v>
       </c>
@@ -3774,7 +3936,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>163</v>
       </c>
@@ -3782,7 +3944,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>164</v>
       </c>
@@ -3790,7 +3952,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>165</v>
       </c>
@@ -3798,7 +3960,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>166</v>
       </c>
@@ -3806,7 +3968,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>167</v>
       </c>
@@ -3814,7 +3976,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>168</v>
       </c>
@@ -3822,7 +3984,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>5</v>
       </c>
@@ -3830,7 +3992,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>170</v>
       </c>
@@ -3838,7 +4000,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>171</v>
       </c>
@@ -3846,7 +4008,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>172</v>
       </c>
@@ -3854,7 +4016,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>173</v>
       </c>
@@ -3862,7 +4024,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>174</v>
       </c>
@@ -3870,7 +4032,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>6</v>
       </c>
@@ -3878,7 +4040,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>176</v>
       </c>
@@ -3886,7 +4048,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>177</v>
       </c>
@@ -3894,7 +4056,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>178</v>
       </c>
@@ -3902,7 +4064,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
         <v>7</v>
       </c>
@@ -3910,7 +4072,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>179</v>
       </c>
@@ -3918,7 +4080,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>180</v>
       </c>
@@ -3926,7 +4088,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>181</v>
       </c>
@@ -3947,28 +4109,28 @@
       <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="123.83203125" style="16" customWidth="1"/>
-    <col min="4" max="4" width="45.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="123.85546875" style="16" customWidth="1"/>
+    <col min="4" max="4" width="45.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B2" s="16" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B3" s="16" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="20" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="32"/>
       <c r="B6" s="57" t="s">
         <v>74</v>
@@ -3976,7 +4138,7 @@
       <c r="C6" s="32"/>
       <c r="D6" s="32"/>
     </row>
-    <row r="7" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="58" t="s">
         <v>84</v>
       </c>
@@ -3988,7 +4150,7 @@
       </c>
       <c r="D7" s="32"/>
     </row>
-    <row r="8" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="58" t="s">
         <v>85</v>
       </c>
@@ -4000,7 +4162,7 @@
       </c>
       <c r="D8" s="32"/>
     </row>
-    <row r="9" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="58" t="s">
         <v>86</v>
       </c>
@@ -4012,7 +4174,7 @@
       </c>
       <c r="D9" s="32"/>
     </row>
-    <row r="10" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="58" t="s">
         <v>87</v>
       </c>
@@ -4024,7 +4186,7 @@
       </c>
       <c r="D10" s="32"/>
     </row>
-    <row r="11" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="58" t="s">
         <v>88</v>
       </c>
@@ -4038,7 +4200,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="58" t="s">
         <v>89</v>
       </c>
@@ -4052,7 +4214,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="58" t="s">
         <v>90</v>
       </c>
@@ -4064,7 +4226,7 @@
       </c>
       <c r="D13" s="32"/>
     </row>
-    <row r="14" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="58" t="s">
         <v>91</v>
       </c>
@@ -4078,7 +4240,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="58" t="s">
         <v>92</v>
       </c>
@@ -4090,7 +4252,7 @@
       </c>
       <c r="D15" s="32"/>
     </row>
-    <row r="16" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="59" t="s">
         <v>93</v>
       </c>
@@ -4104,7 +4266,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="58" t="s">
         <v>94</v>
       </c>
@@ -4116,7 +4278,7 @@
       </c>
       <c r="D17" s="32"/>
     </row>
-    <row r="18" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="58" t="s">
         <v>95</v>
       </c>
@@ -4128,7 +4290,7 @@
       </c>
       <c r="D18" s="32"/>
     </row>
-    <row r="19" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="59" t="s">
         <v>96</v>
       </c>
@@ -4142,7 +4304,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="60" t="s">
         <v>97</v>
       </c>
@@ -4156,7 +4318,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="61" t="s">
         <v>98</v>
       </c>
@@ -4170,7 +4332,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="58" t="s">
         <v>99</v>
       </c>
@@ -4184,7 +4346,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="58" t="s">
         <v>100</v>
       </c>
@@ -4196,7 +4358,7 @@
       </c>
       <c r="D23" s="32"/>
     </row>
-    <row r="24" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="58" t="s">
         <v>101</v>
       </c>
@@ -4210,7 +4372,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="58" t="s">
         <v>102</v>
       </c>
@@ -4224,7 +4386,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
     </row>
   </sheetData>
@@ -4243,15 +4405,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100DD38B4BA879657459FE8C7022D55B717" ma:contentTypeVersion="15" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="d5c0f8514766e5ee81dc36ef583fe1d6">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns3="b91bfc96-29e1-4fce-b1c9-d4ca10ce5a83" xmlns:ns4="924d9142-22e9-433f-95fb-5e56abb45a2b" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5fda3cd559eb82edd80343133af36ddc" ns1:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -4491,7 +4644,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -4500,25 +4653,16 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{23051A02-7089-4210-AA65-89A037B4756D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="924d9142-22e9-433f-95fb-5e56abb45a2b"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="b91bfc96-29e1-4fce-b1c9-d4ca10ce5a83"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{49F939F1-ED95-4D2C-BE48-5C311B9F9B9B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4538,10 +4682,28 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8CC5B40C-D9DA-48AF-AAFA-80EF387CF828}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{23051A02-7089-4210-AA65-89A037B4756D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="b91bfc96-29e1-4fce-b1c9-d4ca10ce5a83"/>
+    <ds:schemaRef ds:uri="924d9142-22e9-433f-95fb-5e56abb45a2b"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
update backlog, auto eval  + test cryptage mdp
</commit_message>
<xml_diff>
--- a/Documents/0-Consignes/Evaluation Gr29.xlsx
+++ b/Documents/0-Consignes/Evaluation Gr29.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Web2.0\Documents\0-Consignes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBD0ACB3-D7D9-4AB4-8CDF-7F23A2367BE5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BDF6B15-408A-447C-A35D-193F6D53BF90}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -830,17 +830,29 @@
     <t>Voulait cliquable au lieu de bouton</t>
   </si>
   <si>
-    <t>Installation
-Sécurité</t>
-  </si>
-  <si>
     <t>Pas de merge car mauvais code
 Attend Gael</t>
   </si>
   <si>
-    <t>https
+    <r>
+      <t xml:space="preserve">https
 pattern
-token</t>
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>token</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Installation
+</t>
   </si>
 </sst>
 </file>
@@ -1414,161 +1426,161 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1873,8 +1885,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A66" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H83" sqref="H83"/>
+    <sheetView tabSelected="1" topLeftCell="A56" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I65" sqref="I65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1937,22 +1949,22 @@
       <c r="E3" s="14"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="90" t="s">
+      <c r="A4" s="107" t="s">
         <v>145</v>
       </c>
-      <c r="B4" s="84" t="s">
+      <c r="B4" s="106" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="79">
+      <c r="C4" s="114">
         <v>-4</v>
       </c>
-      <c r="D4" s="80">
-        <v>0</v>
-      </c>
-      <c r="E4" s="81">
+      <c r="D4" s="121">
+        <v>0</v>
+      </c>
+      <c r="E4" s="122">
         <v>3</v>
       </c>
-      <c r="F4" s="95"/>
+      <c r="F4" s="93"/>
       <c r="G4" s="36" t="s">
         <v>0</v>
       </c>
@@ -1964,12 +1976,12 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="86"/>
-      <c r="B5" s="85"/>
-      <c r="C5" s="73"/>
-      <c r="D5" s="75"/>
-      <c r="E5" s="77"/>
-      <c r="F5" s="96"/>
+      <c r="A5" s="101"/>
+      <c r="B5" s="102"/>
+      <c r="C5" s="115"/>
+      <c r="D5" s="117"/>
+      <c r="E5" s="118"/>
+      <c r="F5" s="94"/>
       <c r="G5" s="33" t="s">
         <v>1</v>
       </c>
@@ -1978,12 +1990,12 @@
       </c>
     </row>
     <row r="6" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="86"/>
-      <c r="B6" s="85"/>
-      <c r="C6" s="73"/>
-      <c r="D6" s="75"/>
-      <c r="E6" s="77"/>
-      <c r="F6" s="97"/>
+      <c r="A6" s="101"/>
+      <c r="B6" s="102"/>
+      <c r="C6" s="115"/>
+      <c r="D6" s="117"/>
+      <c r="E6" s="118"/>
+      <c r="F6" s="83"/>
       <c r="G6" s="35" t="s">
         <v>2</v>
       </c>
@@ -1992,22 +2004,22 @@
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="86" t="s">
+      <c r="A7" s="101" t="s">
         <v>144</v>
       </c>
-      <c r="B7" s="85" t="s">
+      <c r="B7" s="102" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="73">
+      <c r="C7" s="115">
         <v>-4</v>
       </c>
-      <c r="D7" s="75">
-        <v>0</v>
-      </c>
-      <c r="E7" s="77">
+      <c r="D7" s="117">
+        <v>0</v>
+      </c>
+      <c r="E7" s="118">
         <v>1</v>
       </c>
-      <c r="F7" s="98"/>
+      <c r="F7" s="72"/>
       <c r="G7" s="31" t="s">
         <v>0</v>
       </c>
@@ -2022,12 +2034,12 @@
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="86"/>
-      <c r="B8" s="85"/>
-      <c r="C8" s="73"/>
-      <c r="D8" s="75"/>
-      <c r="E8" s="77"/>
-      <c r="F8" s="99"/>
+      <c r="A8" s="101"/>
+      <c r="B8" s="102"/>
+      <c r="C8" s="115"/>
+      <c r="D8" s="117"/>
+      <c r="E8" s="118"/>
+      <c r="F8" s="75"/>
       <c r="G8" s="33" t="s">
         <v>1</v>
       </c>
@@ -2036,12 +2048,12 @@
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="86"/>
-      <c r="B9" s="85"/>
-      <c r="C9" s="73"/>
-      <c r="D9" s="75"/>
-      <c r="E9" s="77"/>
-      <c r="F9" s="100"/>
+      <c r="A9" s="101"/>
+      <c r="B9" s="102"/>
+      <c r="C9" s="115"/>
+      <c r="D9" s="117"/>
+      <c r="E9" s="118"/>
+      <c r="F9" s="76"/>
       <c r="G9" s="35" t="s">
         <v>2</v>
       </c>
@@ -2050,22 +2062,22 @@
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="86" t="s">
+      <c r="A10" s="101" t="s">
         <v>146</v>
       </c>
-      <c r="B10" s="85" t="s">
+      <c r="B10" s="102" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="73">
+      <c r="C10" s="115">
         <v>-1</v>
       </c>
-      <c r="D10" s="75">
-        <v>0</v>
-      </c>
-      <c r="E10" s="77" t="s">
+      <c r="D10" s="117">
+        <v>0</v>
+      </c>
+      <c r="E10" s="118" t="s">
         <v>185</v>
       </c>
-      <c r="F10" s="98"/>
+      <c r="F10" s="72"/>
       <c r="G10" s="31" t="s">
         <v>0</v>
       </c>
@@ -2077,12 +2089,12 @@
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="86"/>
-      <c r="B11" s="85"/>
-      <c r="C11" s="73"/>
-      <c r="D11" s="75"/>
-      <c r="E11" s="77"/>
-      <c r="F11" s="100"/>
+      <c r="A11" s="101"/>
+      <c r="B11" s="102"/>
+      <c r="C11" s="115"/>
+      <c r="D11" s="117"/>
+      <c r="E11" s="118"/>
+      <c r="F11" s="76"/>
       <c r="G11" s="33" t="s">
         <v>1</v>
       </c>
@@ -2091,22 +2103,22 @@
       </c>
     </row>
     <row r="12" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="87" t="s">
+      <c r="A12" s="103" t="s">
         <v>147</v>
       </c>
-      <c r="B12" s="85" t="s">
+      <c r="B12" s="102" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="73">
+      <c r="C12" s="115">
         <v>-4</v>
       </c>
-      <c r="D12" s="75">
-        <v>0</v>
-      </c>
-      <c r="E12" s="77" t="s">
+      <c r="D12" s="117">
+        <v>0</v>
+      </c>
+      <c r="E12" s="118" t="s">
         <v>185</v>
       </c>
-      <c r="F12" s="98"/>
+      <c r="F12" s="72"/>
       <c r="G12" s="31" t="s">
         <v>0</v>
       </c>
@@ -2118,12 +2130,12 @@
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="87"/>
-      <c r="B13" s="85"/>
-      <c r="C13" s="73"/>
-      <c r="D13" s="75"/>
-      <c r="E13" s="77"/>
-      <c r="F13" s="100"/>
+      <c r="A13" s="103"/>
+      <c r="B13" s="102"/>
+      <c r="C13" s="115"/>
+      <c r="D13" s="117"/>
+      <c r="E13" s="118"/>
+      <c r="F13" s="76"/>
       <c r="G13" s="33" t="s">
         <v>1</v>
       </c>
@@ -2132,22 +2144,22 @@
       </c>
     </row>
     <row r="14" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A14" s="83" t="s">
+      <c r="A14" s="108" t="s">
         <v>148</v>
       </c>
-      <c r="B14" s="85" t="s">
+      <c r="B14" s="102" t="s">
         <v>139</v>
       </c>
-      <c r="C14" s="73" t="s">
+      <c r="C14" s="115" t="s">
         <v>185</v>
       </c>
-      <c r="D14" s="75" t="s">
+      <c r="D14" s="117" t="s">
         <v>185</v>
       </c>
-      <c r="E14" s="77">
+      <c r="E14" s="118">
         <v>2</v>
       </c>
-      <c r="F14" s="101"/>
+      <c r="F14" s="82"/>
       <c r="G14" s="35" t="s">
         <v>2</v>
       </c>
@@ -2156,24 +2168,24 @@
       </c>
     </row>
     <row r="15" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A15" s="83"/>
-      <c r="B15" s="85"/>
-      <c r="C15" s="73"/>
-      <c r="D15" s="75"/>
-      <c r="E15" s="77"/>
-      <c r="F15" s="96"/>
+      <c r="A15" s="108"/>
+      <c r="B15" s="102"/>
+      <c r="C15" s="115"/>
+      <c r="D15" s="117"/>
+      <c r="E15" s="118"/>
+      <c r="F15" s="94"/>
       <c r="G15" s="35"/>
       <c r="H15" s="38" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="91"/>
-      <c r="B16" s="89"/>
-      <c r="C16" s="74"/>
-      <c r="D16" s="76"/>
-      <c r="E16" s="78"/>
-      <c r="F16" s="102"/>
+      <c r="A16" s="109"/>
+      <c r="B16" s="110"/>
+      <c r="C16" s="116"/>
+      <c r="D16" s="119"/>
+      <c r="E16" s="120"/>
+      <c r="F16" s="95"/>
       <c r="G16" s="39"/>
       <c r="H16" s="40" t="s">
         <v>140</v>
@@ -2200,22 +2212,22 @@
       <c r="F18" s="65"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="90" t="s">
+      <c r="A19" s="107" t="s">
         <v>150</v>
       </c>
-      <c r="B19" s="84" t="s">
+      <c r="B19" s="106" t="s">
         <v>115</v>
       </c>
-      <c r="C19" s="79">
+      <c r="C19" s="114">
         <v>-1</v>
       </c>
-      <c r="D19" s="80">
-        <v>0</v>
-      </c>
-      <c r="E19" s="81">
-        <v>0</v>
-      </c>
-      <c r="F19" s="103">
+      <c r="D19" s="121">
+        <v>0</v>
+      </c>
+      <c r="E19" s="122">
+        <v>0</v>
+      </c>
+      <c r="F19" s="96">
         <v>0</v>
       </c>
       <c r="G19" s="36" t="s">
@@ -2232,12 +2244,12 @@
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="86"/>
-      <c r="B20" s="85"/>
-      <c r="C20" s="73"/>
-      <c r="D20" s="75"/>
-      <c r="E20" s="77"/>
-      <c r="F20" s="104"/>
+      <c r="A20" s="101"/>
+      <c r="B20" s="102"/>
+      <c r="C20" s="115"/>
+      <c r="D20" s="117"/>
+      <c r="E20" s="118"/>
+      <c r="F20" s="78"/>
       <c r="G20" s="33" t="s">
         <v>1</v>
       </c>
@@ -2246,22 +2258,22 @@
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="86" t="s">
+      <c r="A21" s="101" t="s">
         <v>151</v>
       </c>
-      <c r="B21" s="85" t="s">
+      <c r="B21" s="102" t="s">
         <v>114</v>
       </c>
-      <c r="C21" s="73">
+      <c r="C21" s="115">
         <v>-2</v>
       </c>
-      <c r="D21" s="75">
-        <v>0</v>
-      </c>
-      <c r="E21" s="77">
+      <c r="D21" s="117">
+        <v>0</v>
+      </c>
+      <c r="E21" s="118">
         <v>1</v>
       </c>
-      <c r="F21" s="105">
+      <c r="F21" s="97">
         <v>1</v>
       </c>
       <c r="G21" s="31" t="s">
@@ -2278,12 +2290,12 @@
       </c>
     </row>
     <row r="22" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="86"/>
-      <c r="B22" s="85"/>
-      <c r="C22" s="73"/>
-      <c r="D22" s="75"/>
-      <c r="E22" s="77"/>
-      <c r="F22" s="106"/>
+      <c r="A22" s="101"/>
+      <c r="B22" s="102"/>
+      <c r="C22" s="115"/>
+      <c r="D22" s="117"/>
+      <c r="E22" s="118"/>
+      <c r="F22" s="98"/>
       <c r="G22" s="33" t="s">
         <v>1</v>
       </c>
@@ -2292,12 +2304,12 @@
       </c>
     </row>
     <row r="23" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A23" s="86"/>
-      <c r="B23" s="85"/>
-      <c r="C23" s="73"/>
-      <c r="D23" s="75"/>
-      <c r="E23" s="77"/>
-      <c r="F23" s="107"/>
+      <c r="A23" s="101"/>
+      <c r="B23" s="102"/>
+      <c r="C23" s="115"/>
+      <c r="D23" s="117"/>
+      <c r="E23" s="118"/>
+      <c r="F23" s="99"/>
       <c r="G23" s="35" t="s">
         <v>2</v>
       </c>
@@ -2306,22 +2318,22 @@
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="86" t="s">
+      <c r="A24" s="101" t="s">
         <v>152</v>
       </c>
-      <c r="B24" s="85" t="s">
+      <c r="B24" s="102" t="s">
         <v>22</v>
       </c>
-      <c r="C24" s="73">
+      <c r="C24" s="115">
         <v>-3</v>
       </c>
-      <c r="D24" s="75">
-        <v>0</v>
-      </c>
-      <c r="E24" s="77" t="s">
+      <c r="D24" s="117">
+        <v>0</v>
+      </c>
+      <c r="E24" s="118" t="s">
         <v>185</v>
       </c>
-      <c r="F24" s="108">
+      <c r="F24" s="77">
         <v>0</v>
       </c>
       <c r="G24" s="31" t="s">
@@ -2338,12 +2350,12 @@
       </c>
     </row>
     <row r="25" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A25" s="86"/>
-      <c r="B25" s="85"/>
-      <c r="C25" s="73"/>
-      <c r="D25" s="75"/>
-      <c r="E25" s="77"/>
-      <c r="F25" s="104"/>
+      <c r="A25" s="101"/>
+      <c r="B25" s="102"/>
+      <c r="C25" s="115"/>
+      <c r="D25" s="117"/>
+      <c r="E25" s="118"/>
+      <c r="F25" s="78"/>
       <c r="G25" s="33" t="s">
         <v>1</v>
       </c>
@@ -2355,22 +2367,22 @@
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="86" t="s">
+      <c r="A26" s="101" t="s">
         <v>153</v>
       </c>
-      <c r="B26" s="85" t="s">
+      <c r="B26" s="102" t="s">
         <v>24</v>
       </c>
-      <c r="C26" s="73">
+      <c r="C26" s="115">
         <v>-2</v>
       </c>
-      <c r="D26" s="75">
-        <v>0</v>
-      </c>
-      <c r="E26" s="77" t="s">
+      <c r="D26" s="117">
+        <v>0</v>
+      </c>
+      <c r="E26" s="118" t="s">
         <v>185</v>
       </c>
-      <c r="F26" s="108">
+      <c r="F26" s="77">
         <v>0</v>
       </c>
       <c r="G26" s="31" t="s">
@@ -2384,12 +2396,12 @@
       </c>
     </row>
     <row r="27" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="88"/>
-      <c r="B27" s="89"/>
-      <c r="C27" s="74"/>
-      <c r="D27" s="76"/>
-      <c r="E27" s="78"/>
-      <c r="F27" s="109"/>
+      <c r="A27" s="111"/>
+      <c r="B27" s="110"/>
+      <c r="C27" s="116"/>
+      <c r="D27" s="119"/>
+      <c r="E27" s="120"/>
+      <c r="F27" s="100"/>
       <c r="G27" s="42" t="s">
         <v>1</v>
       </c>
@@ -2418,22 +2430,22 @@
       <c r="F29" s="65"/>
     </row>
     <row r="30" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="92" t="s">
+      <c r="A30" s="112" t="s">
         <v>155</v>
       </c>
-      <c r="B30" s="84" t="s">
+      <c r="B30" s="106" t="s">
         <v>28</v>
       </c>
-      <c r="C30" s="79">
+      <c r="C30" s="114">
         <v>-10</v>
       </c>
-      <c r="D30" s="80">
-        <v>0</v>
-      </c>
-      <c r="E30" s="81">
+      <c r="D30" s="121">
+        <v>0</v>
+      </c>
+      <c r="E30" s="122">
         <v>1</v>
       </c>
-      <c r="F30" s="110"/>
+      <c r="F30" s="84"/>
       <c r="G30" s="36" t="s">
         <v>0</v>
       </c>
@@ -2441,19 +2453,19 @@
         <v>29</v>
       </c>
       <c r="I30" s="16" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="J30" t="s">
         <v>243</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" s="87"/>
-      <c r="B31" s="85"/>
-      <c r="C31" s="73"/>
-      <c r="D31" s="75"/>
-      <c r="E31" s="77"/>
-      <c r="F31" s="111"/>
+      <c r="A31" s="103"/>
+      <c r="B31" s="102"/>
+      <c r="C31" s="115"/>
+      <c r="D31" s="117"/>
+      <c r="E31" s="118"/>
+      <c r="F31" s="80"/>
       <c r="G31" s="33" t="s">
         <v>1</v>
       </c>
@@ -2462,12 +2474,12 @@
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32" s="87"/>
-      <c r="B32" s="85"/>
-      <c r="C32" s="73"/>
-      <c r="D32" s="75"/>
-      <c r="E32" s="77"/>
-      <c r="F32" s="112"/>
+      <c r="A32" s="103"/>
+      <c r="B32" s="102"/>
+      <c r="C32" s="115"/>
+      <c r="D32" s="117"/>
+      <c r="E32" s="118"/>
+      <c r="F32" s="85"/>
       <c r="G32" s="35" t="s">
         <v>2</v>
       </c>
@@ -2476,22 +2488,22 @@
       </c>
     </row>
     <row r="33" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A33" s="86" t="s">
+      <c r="A33" s="101" t="s">
         <v>156</v>
       </c>
-      <c r="B33" s="85" t="s">
+      <c r="B33" s="102" t="s">
         <v>32</v>
       </c>
-      <c r="C33" s="73">
+      <c r="C33" s="115">
         <v>-20</v>
       </c>
-      <c r="D33" s="75">
-        <v>0</v>
-      </c>
-      <c r="E33" s="77">
+      <c r="D33" s="117">
+        <v>0</v>
+      </c>
+      <c r="E33" s="118">
         <v>1</v>
       </c>
-      <c r="F33" s="113">
+      <c r="F33" s="86">
         <v>0.25</v>
       </c>
       <c r="G33" s="31" t="s">
@@ -2504,16 +2516,16 @@
         <v>244</v>
       </c>
       <c r="K33" s="16" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="34" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A34" s="86"/>
-      <c r="B34" s="85"/>
-      <c r="C34" s="73"/>
-      <c r="D34" s="75"/>
-      <c r="E34" s="77"/>
-      <c r="F34" s="114"/>
+      <c r="A34" s="101"/>
+      <c r="B34" s="102"/>
+      <c r="C34" s="115"/>
+      <c r="D34" s="117"/>
+      <c r="E34" s="118"/>
+      <c r="F34" s="87"/>
       <c r="G34" s="33" t="s">
         <v>1</v>
       </c>
@@ -2522,12 +2534,12 @@
       </c>
     </row>
     <row r="35" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A35" s="86"/>
-      <c r="B35" s="85"/>
-      <c r="C35" s="73"/>
-      <c r="D35" s="75"/>
-      <c r="E35" s="77"/>
-      <c r="F35" s="115"/>
+      <c r="A35" s="101"/>
+      <c r="B35" s="102"/>
+      <c r="C35" s="115"/>
+      <c r="D35" s="117"/>
+      <c r="E35" s="118"/>
+      <c r="F35" s="88"/>
       <c r="G35" s="35" t="s">
         <v>2</v>
       </c>
@@ -2536,22 +2548,22 @@
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A36" s="86" t="s">
+      <c r="A36" s="101" t="s">
         <v>157</v>
       </c>
-      <c r="B36" s="85" t="s">
+      <c r="B36" s="102" t="s">
         <v>35</v>
       </c>
-      <c r="C36" s="73">
+      <c r="C36" s="115">
         <v>-2</v>
       </c>
-      <c r="D36" s="75">
-        <v>0</v>
-      </c>
-      <c r="E36" s="77" t="s">
+      <c r="D36" s="117">
+        <v>0</v>
+      </c>
+      <c r="E36" s="118" t="s">
         <v>185</v>
       </c>
-      <c r="F36" s="108">
+      <c r="F36" s="77">
         <v>0</v>
       </c>
       <c r="G36" s="31" t="s">
@@ -2565,12 +2577,12 @@
       </c>
     </row>
     <row r="37" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A37" s="86"/>
-      <c r="B37" s="85"/>
-      <c r="C37" s="73"/>
-      <c r="D37" s="75"/>
-      <c r="E37" s="77"/>
-      <c r="F37" s="104"/>
+      <c r="A37" s="101"/>
+      <c r="B37" s="102"/>
+      <c r="C37" s="115"/>
+      <c r="D37" s="117"/>
+      <c r="E37" s="118"/>
+      <c r="F37" s="78"/>
       <c r="G37" s="33" t="s">
         <v>1</v>
       </c>
@@ -2661,22 +2673,22 @@
       <c r="F41" s="65"/>
     </row>
     <row r="42" spans="1:11" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="93" t="s">
+      <c r="A42" s="104" t="s">
         <v>161</v>
       </c>
-      <c r="B42" s="84" t="s">
+      <c r="B42" s="106" t="s">
         <v>109</v>
       </c>
-      <c r="C42" s="79">
+      <c r="C42" s="114">
         <v>-1</v>
       </c>
-      <c r="D42" s="80">
-        <v>0</v>
-      </c>
-      <c r="E42" s="81" t="s">
+      <c r="D42" s="121">
+        <v>0</v>
+      </c>
+      <c r="E42" s="122" t="s">
         <v>185</v>
       </c>
-      <c r="F42" s="116">
+      <c r="F42" s="89">
         <v>-0.25</v>
       </c>
       <c r="G42" s="36" t="s">
@@ -2688,42 +2700,42 @@
       <c r="I42" t="s">
         <v>205</v>
       </c>
-      <c r="J42" s="72" t="s">
+      <c r="J42" s="123" t="s">
         <v>247</v>
       </c>
     </row>
     <row r="43" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A43" s="94"/>
-      <c r="B43" s="85"/>
-      <c r="C43" s="73"/>
-      <c r="D43" s="75"/>
-      <c r="E43" s="77"/>
-      <c r="F43" s="117"/>
+      <c r="A43" s="105"/>
+      <c r="B43" s="102"/>
+      <c r="C43" s="115"/>
+      <c r="D43" s="117"/>
+      <c r="E43" s="118"/>
+      <c r="F43" s="90"/>
       <c r="G43" s="33" t="s">
         <v>1</v>
       </c>
       <c r="H43" s="38" t="s">
         <v>42</v>
       </c>
-      <c r="J43" s="72"/>
+      <c r="J43" s="123"/>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A44" s="87" t="s">
+      <c r="A44" s="103" t="s">
         <v>162</v>
       </c>
-      <c r="B44" s="85" t="s">
+      <c r="B44" s="102" t="s">
         <v>188</v>
       </c>
-      <c r="C44" s="73">
+      <c r="C44" s="115">
         <v>-1</v>
       </c>
-      <c r="D44" s="75">
-        <v>0</v>
-      </c>
-      <c r="E44" s="77" t="s">
+      <c r="D44" s="117">
+        <v>0</v>
+      </c>
+      <c r="E44" s="118" t="s">
         <v>185</v>
       </c>
-      <c r="F44" s="108">
+      <c r="F44" s="77">
         <v>0</v>
       </c>
       <c r="G44" s="31" t="s">
@@ -2740,12 +2752,12 @@
       </c>
     </row>
     <row r="45" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A45" s="87"/>
-      <c r="B45" s="85"/>
-      <c r="C45" s="73"/>
-      <c r="D45" s="75"/>
-      <c r="E45" s="77"/>
-      <c r="F45" s="104"/>
+      <c r="A45" s="103"/>
+      <c r="B45" s="102"/>
+      <c r="C45" s="115"/>
+      <c r="D45" s="117"/>
+      <c r="E45" s="118"/>
+      <c r="F45" s="78"/>
       <c r="G45" s="33" t="s">
         <v>1</v>
       </c>
@@ -2760,22 +2772,22 @@
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A46" s="86" t="s">
+      <c r="A46" s="101" t="s">
         <v>163</v>
       </c>
-      <c r="B46" s="85" t="s">
+      <c r="B46" s="102" t="s">
         <v>122</v>
       </c>
-      <c r="C46" s="73">
+      <c r="C46" s="115">
         <v>-1</v>
       </c>
-      <c r="D46" s="75">
-        <v>0</v>
-      </c>
-      <c r="E46" s="77" t="s">
+      <c r="D46" s="117">
+        <v>0</v>
+      </c>
+      <c r="E46" s="118" t="s">
         <v>185</v>
       </c>
-      <c r="F46" s="108">
+      <c r="F46" s="77">
         <v>0</v>
       </c>
       <c r="G46" s="31" t="s">
@@ -2789,12 +2801,12 @@
       </c>
     </row>
     <row r="47" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A47" s="86"/>
-      <c r="B47" s="85"/>
-      <c r="C47" s="73"/>
-      <c r="D47" s="75"/>
-      <c r="E47" s="77"/>
-      <c r="F47" s="104"/>
+      <c r="A47" s="101"/>
+      <c r="B47" s="102"/>
+      <c r="C47" s="115"/>
+      <c r="D47" s="117"/>
+      <c r="E47" s="118"/>
+      <c r="F47" s="78"/>
       <c r="G47" s="33" t="s">
         <v>1</v>
       </c>
@@ -2806,22 +2818,22 @@
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A48" s="86" t="s">
+      <c r="A48" s="101" t="s">
         <v>164</v>
       </c>
-      <c r="B48" s="85" t="s">
+      <c r="B48" s="102" t="s">
         <v>119</v>
       </c>
-      <c r="C48" s="73">
+      <c r="C48" s="115">
         <v>-1</v>
       </c>
-      <c r="D48" s="75">
-        <v>0</v>
-      </c>
-      <c r="E48" s="77" t="s">
+      <c r="D48" s="117">
+        <v>0</v>
+      </c>
+      <c r="E48" s="118" t="s">
         <v>185</v>
       </c>
-      <c r="F48" s="118">
+      <c r="F48" s="79">
         <v>-0.25</v>
       </c>
       <c r="G48" s="31" t="s">
@@ -2836,12 +2848,12 @@
       </c>
     </row>
     <row r="49" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A49" s="86"/>
-      <c r="B49" s="85"/>
-      <c r="C49" s="73"/>
-      <c r="D49" s="75"/>
-      <c r="E49" s="77"/>
-      <c r="F49" s="112"/>
+      <c r="A49" s="101"/>
+      <c r="B49" s="102"/>
+      <c r="C49" s="115"/>
+      <c r="D49" s="117"/>
+      <c r="E49" s="118"/>
+      <c r="F49" s="85"/>
       <c r="G49" s="33" t="s">
         <v>1</v>
       </c>
@@ -2853,22 +2865,22 @@
       </c>
     </row>
     <row r="50" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A50" s="87" t="s">
+      <c r="A50" s="103" t="s">
         <v>165</v>
       </c>
-      <c r="B50" s="85" t="s">
+      <c r="B50" s="102" t="s">
         <v>120</v>
       </c>
-      <c r="C50" s="73">
+      <c r="C50" s="115">
         <v>-1</v>
       </c>
-      <c r="D50" s="75">
-        <v>0</v>
-      </c>
-      <c r="E50" s="77" t="s">
+      <c r="D50" s="117">
+        <v>0</v>
+      </c>
+      <c r="E50" s="118" t="s">
         <v>185</v>
       </c>
-      <c r="F50" s="119">
+      <c r="F50" s="91">
         <v>0</v>
       </c>
       <c r="G50" s="31" t="s">
@@ -2885,12 +2897,12 @@
       </c>
     </row>
     <row r="51" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A51" s="87"/>
-      <c r="B51" s="85"/>
-      <c r="C51" s="73"/>
-      <c r="D51" s="75"/>
-      <c r="E51" s="77"/>
-      <c r="F51" s="120"/>
+      <c r="A51" s="103"/>
+      <c r="B51" s="102"/>
+      <c r="C51" s="115"/>
+      <c r="D51" s="117"/>
+      <c r="E51" s="118"/>
+      <c r="F51" s="92"/>
       <c r="G51" s="33" t="s">
         <v>1</v>
       </c>
@@ -2899,22 +2911,22 @@
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A52" s="86" t="s">
+      <c r="A52" s="101" t="s">
         <v>166</v>
       </c>
-      <c r="B52" s="85" t="s">
+      <c r="B52" s="102" t="s">
         <v>49</v>
       </c>
-      <c r="C52" s="73">
+      <c r="C52" s="115">
         <v>-1</v>
       </c>
-      <c r="D52" s="75">
-        <v>0</v>
-      </c>
-      <c r="E52" s="77" t="s">
+      <c r="D52" s="117">
+        <v>0</v>
+      </c>
+      <c r="E52" s="118" t="s">
         <v>185</v>
       </c>
-      <c r="F52" s="108">
+      <c r="F52" s="77">
         <v>0</v>
       </c>
       <c r="G52" s="31" t="s">
@@ -2928,12 +2940,12 @@
       </c>
     </row>
     <row r="53" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A53" s="86"/>
-      <c r="B53" s="85"/>
-      <c r="C53" s="73"/>
-      <c r="D53" s="75"/>
-      <c r="E53" s="77"/>
-      <c r="F53" s="104"/>
+      <c r="A53" s="101"/>
+      <c r="B53" s="102"/>
+      <c r="C53" s="115"/>
+      <c r="D53" s="117"/>
+      <c r="E53" s="118"/>
+      <c r="F53" s="78"/>
       <c r="G53" s="33" t="s">
         <v>1</v>
       </c>
@@ -2945,22 +2957,22 @@
       </c>
     </row>
     <row r="54" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A54" s="86" t="s">
+      <c r="A54" s="101" t="s">
         <v>167</v>
       </c>
-      <c r="B54" s="85" t="s">
+      <c r="B54" s="102" t="s">
         <v>52</v>
       </c>
-      <c r="C54" s="73">
+      <c r="C54" s="115">
         <v>-2</v>
       </c>
-      <c r="D54" s="75">
-        <v>0</v>
-      </c>
-      <c r="E54" s="77" t="s">
+      <c r="D54" s="117">
+        <v>0</v>
+      </c>
+      <c r="E54" s="118" t="s">
         <v>185</v>
       </c>
-      <c r="F54" s="108">
+      <c r="F54" s="77">
         <v>0</v>
       </c>
       <c r="G54" s="31" t="s">
@@ -2974,12 +2986,12 @@
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A55" s="86"/>
-      <c r="B55" s="85"/>
-      <c r="C55" s="73"/>
-      <c r="D55" s="75"/>
-      <c r="E55" s="77"/>
-      <c r="F55" s="104"/>
+      <c r="A55" s="101"/>
+      <c r="B55" s="102"/>
+      <c r="C55" s="115"/>
+      <c r="D55" s="117"/>
+      <c r="E55" s="118"/>
+      <c r="F55" s="78"/>
       <c r="G55" s="33" t="s">
         <v>1</v>
       </c>
@@ -2991,22 +3003,22 @@
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A56" s="83" t="s">
+      <c r="A56" s="108" t="s">
         <v>168</v>
       </c>
-      <c r="B56" s="85" t="s">
+      <c r="B56" s="102" t="s">
         <v>53</v>
       </c>
-      <c r="C56" s="73">
+      <c r="C56" s="115">
         <v>-2</v>
       </c>
-      <c r="D56" s="75">
-        <v>0</v>
-      </c>
-      <c r="E56" s="77">
+      <c r="D56" s="117">
+        <v>0</v>
+      </c>
+      <c r="E56" s="118">
         <v>1</v>
       </c>
-      <c r="F56" s="118"/>
+      <c r="F56" s="79"/>
       <c r="G56" s="31" t="s">
         <v>0</v>
       </c>
@@ -3021,12 +3033,12 @@
       </c>
     </row>
     <row r="57" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A57" s="83"/>
-      <c r="B57" s="85"/>
-      <c r="C57" s="73"/>
-      <c r="D57" s="75"/>
-      <c r="E57" s="77"/>
-      <c r="F57" s="111"/>
+      <c r="A57" s="108"/>
+      <c r="B57" s="102"/>
+      <c r="C57" s="115"/>
+      <c r="D57" s="117"/>
+      <c r="E57" s="118"/>
+      <c r="F57" s="80"/>
       <c r="G57" s="33" t="s">
         <v>1</v>
       </c>
@@ -3035,12 +3047,12 @@
       </c>
     </row>
     <row r="58" spans="1:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="91"/>
-      <c r="B58" s="89"/>
-      <c r="C58" s="74"/>
-      <c r="D58" s="76"/>
-      <c r="E58" s="78"/>
-      <c r="F58" s="123"/>
+      <c r="A58" s="109"/>
+      <c r="B58" s="110"/>
+      <c r="C58" s="116"/>
+      <c r="D58" s="119"/>
+      <c r="E58" s="120"/>
+      <c r="F58" s="81"/>
       <c r="G58" s="39" t="s">
         <v>2</v>
       </c>
@@ -3069,22 +3081,22 @@
       <c r="F60" s="65"/>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A61" s="90" t="s">
+      <c r="A61" s="107" t="s">
         <v>170</v>
       </c>
-      <c r="B61" s="84" t="s">
+      <c r="B61" s="106" t="s">
         <v>40</v>
       </c>
-      <c r="C61" s="79">
+      <c r="C61" s="114">
         <v>-1</v>
       </c>
-      <c r="D61" s="80">
-        <v>0</v>
-      </c>
-      <c r="E61" s="81" t="s">
+      <c r="D61" s="121">
+        <v>0</v>
+      </c>
+      <c r="E61" s="122" t="s">
         <v>185</v>
       </c>
-      <c r="F61" s="122"/>
+      <c r="F61" s="74"/>
       <c r="G61" s="36" t="s">
         <v>0</v>
       </c>
@@ -3096,12 +3108,12 @@
       </c>
     </row>
     <row r="62" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A62" s="86"/>
-      <c r="B62" s="85"/>
-      <c r="C62" s="73"/>
-      <c r="D62" s="75"/>
-      <c r="E62" s="77"/>
-      <c r="F62" s="100"/>
+      <c r="A62" s="101"/>
+      <c r="B62" s="102"/>
+      <c r="C62" s="115"/>
+      <c r="D62" s="117"/>
+      <c r="E62" s="118"/>
+      <c r="F62" s="76"/>
       <c r="G62" s="33" t="s">
         <v>1</v>
       </c>
@@ -3110,22 +3122,22 @@
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A63" s="86" t="s">
+      <c r="A63" s="101" t="s">
         <v>171</v>
       </c>
-      <c r="B63" s="85" t="s">
+      <c r="B63" s="102" t="s">
         <v>57</v>
       </c>
-      <c r="C63" s="73">
+      <c r="C63" s="115">
         <v>-1</v>
       </c>
-      <c r="D63" s="75">
-        <v>0</v>
-      </c>
-      <c r="E63" s="77" t="s">
+      <c r="D63" s="117">
+        <v>0</v>
+      </c>
+      <c r="E63" s="118" t="s">
         <v>185</v>
       </c>
-      <c r="F63" s="101"/>
+      <c r="F63" s="82"/>
       <c r="G63" s="31" t="s">
         <v>0</v>
       </c>
@@ -3137,12 +3149,12 @@
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A64" s="86"/>
-      <c r="B64" s="85"/>
-      <c r="C64" s="73"/>
-      <c r="D64" s="75"/>
-      <c r="E64" s="77"/>
-      <c r="F64" s="97"/>
+      <c r="A64" s="101"/>
+      <c r="B64" s="102"/>
+      <c r="C64" s="115"/>
+      <c r="D64" s="117"/>
+      <c r="E64" s="118"/>
+      <c r="F64" s="83"/>
       <c r="G64" s="33" t="s">
         <v>1</v>
       </c>
@@ -3151,22 +3163,22 @@
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A65" s="86" t="s">
+      <c r="A65" s="101" t="s">
         <v>172</v>
       </c>
-      <c r="B65" s="85" t="s">
+      <c r="B65" s="102" t="s">
         <v>60</v>
       </c>
-      <c r="C65" s="73">
+      <c r="C65" s="115">
         <v>-1</v>
       </c>
-      <c r="D65" s="75">
-        <v>0</v>
-      </c>
-      <c r="E65" s="77" t="s">
+      <c r="D65" s="117">
+        <v>0</v>
+      </c>
+      <c r="E65" s="118" t="s">
         <v>185</v>
       </c>
-      <c r="F65" s="101"/>
+      <c r="F65" s="82"/>
       <c r="G65" s="31" t="s">
         <v>0</v>
       </c>
@@ -3178,12 +3190,12 @@
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A66" s="86"/>
-      <c r="B66" s="85"/>
-      <c r="C66" s="73"/>
-      <c r="D66" s="75"/>
-      <c r="E66" s="77"/>
-      <c r="F66" s="97"/>
+      <c r="A66" s="101"/>
+      <c r="B66" s="102"/>
+      <c r="C66" s="115"/>
+      <c r="D66" s="117"/>
+      <c r="E66" s="118"/>
+      <c r="F66" s="83"/>
       <c r="G66" s="33" t="s">
         <v>1</v>
       </c>
@@ -3192,22 +3204,22 @@
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A67" s="86" t="s">
+      <c r="A67" s="101" t="s">
         <v>173</v>
       </c>
-      <c r="B67" s="85" t="s">
+      <c r="B67" s="102" t="s">
         <v>126</v>
       </c>
-      <c r="C67" s="73">
+      <c r="C67" s="115">
         <v>-1</v>
       </c>
-      <c r="D67" s="75">
-        <v>0</v>
-      </c>
-      <c r="E67" s="77">
+      <c r="D67" s="117">
+        <v>0</v>
+      </c>
+      <c r="E67" s="118">
         <v>1</v>
       </c>
-      <c r="F67" s="98"/>
+      <c r="F67" s="72"/>
       <c r="G67" s="31" t="s">
         <v>0</v>
       </c>
@@ -3219,12 +3231,12 @@
       </c>
     </row>
     <row r="68" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A68" s="86"/>
-      <c r="B68" s="85"/>
-      <c r="C68" s="73"/>
-      <c r="D68" s="75"/>
-      <c r="E68" s="77"/>
-      <c r="F68" s="99"/>
+      <c r="A68" s="101"/>
+      <c r="B68" s="102"/>
+      <c r="C68" s="115"/>
+      <c r="D68" s="117"/>
+      <c r="E68" s="118"/>
+      <c r="F68" s="75"/>
       <c r="G68" s="33" t="s">
         <v>1</v>
       </c>
@@ -3233,12 +3245,12 @@
       </c>
     </row>
     <row r="69" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A69" s="86"/>
-      <c r="B69" s="85"/>
-      <c r="C69" s="73"/>
-      <c r="D69" s="75"/>
-      <c r="E69" s="77"/>
-      <c r="F69" s="100"/>
+      <c r="A69" s="101"/>
+      <c r="B69" s="102"/>
+      <c r="C69" s="115"/>
+      <c r="D69" s="117"/>
+      <c r="E69" s="118"/>
+      <c r="F69" s="76"/>
       <c r="G69" s="35" t="s">
         <v>2</v>
       </c>
@@ -3247,22 +3259,22 @@
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A70" s="86" t="s">
+      <c r="A70" s="101" t="s">
         <v>174</v>
       </c>
-      <c r="B70" s="85" t="s">
+      <c r="B70" s="102" t="s">
         <v>121</v>
       </c>
-      <c r="C70" s="73">
+      <c r="C70" s="115">
         <v>-1</v>
       </c>
-      <c r="D70" s="75">
-        <v>0</v>
-      </c>
-      <c r="E70" s="77" t="s">
+      <c r="D70" s="117">
+        <v>0</v>
+      </c>
+      <c r="E70" s="118" t="s">
         <v>185</v>
       </c>
-      <c r="F70" s="98"/>
+      <c r="F70" s="72"/>
       <c r="G70" s="31" t="s">
         <v>0</v>
       </c>
@@ -3271,12 +3283,12 @@
       </c>
     </row>
     <row r="71" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A71" s="88"/>
-      <c r="B71" s="89"/>
-      <c r="C71" s="74"/>
-      <c r="D71" s="76"/>
-      <c r="E71" s="78"/>
-      <c r="F71" s="121"/>
+      <c r="A71" s="111"/>
+      <c r="B71" s="110"/>
+      <c r="C71" s="116"/>
+      <c r="D71" s="119"/>
+      <c r="E71" s="120"/>
+      <c r="F71" s="73"/>
       <c r="G71" s="42" t="s">
         <v>1</v>
       </c>
@@ -3305,22 +3317,22 @@
       <c r="F73" s="65"/>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A74" s="82" t="s">
+      <c r="A74" s="113" t="s">
         <v>176</v>
       </c>
-      <c r="B74" s="84" t="s">
+      <c r="B74" s="106" t="s">
         <v>66</v>
       </c>
-      <c r="C74" s="79">
+      <c r="C74" s="114">
         <v>-2</v>
       </c>
-      <c r="D74" s="80">
-        <v>0</v>
-      </c>
-      <c r="E74" s="81">
+      <c r="D74" s="121">
+        <v>0</v>
+      </c>
+      <c r="E74" s="122">
         <v>1</v>
       </c>
-      <c r="F74" s="122"/>
+      <c r="F74" s="74"/>
       <c r="G74" s="36" t="s">
         <v>0</v>
       </c>
@@ -3332,12 +3344,12 @@
       </c>
     </row>
     <row r="75" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A75" s="83"/>
-      <c r="B75" s="85"/>
-      <c r="C75" s="73"/>
-      <c r="D75" s="75"/>
-      <c r="E75" s="77"/>
-      <c r="F75" s="99"/>
+      <c r="A75" s="108"/>
+      <c r="B75" s="102"/>
+      <c r="C75" s="115"/>
+      <c r="D75" s="117"/>
+      <c r="E75" s="118"/>
+      <c r="F75" s="75"/>
       <c r="G75" s="33" t="s">
         <v>1</v>
       </c>
@@ -3346,12 +3358,12 @@
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A76" s="83"/>
-      <c r="B76" s="85"/>
-      <c r="C76" s="73"/>
-      <c r="D76" s="75"/>
-      <c r="E76" s="77"/>
-      <c r="F76" s="100"/>
+      <c r="A76" s="108"/>
+      <c r="B76" s="102"/>
+      <c r="C76" s="115"/>
+      <c r="D76" s="117"/>
+      <c r="E76" s="118"/>
+      <c r="F76" s="76"/>
       <c r="G76" s="35" t="s">
         <v>2</v>
       </c>
@@ -3438,22 +3450,22 @@
       <c r="F81" s="65"/>
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A82" s="92" t="s">
+      <c r="A82" s="112" t="s">
         <v>179</v>
       </c>
-      <c r="B82" s="84" t="s">
+      <c r="B82" s="106" t="s">
         <v>132</v>
       </c>
-      <c r="C82" s="79">
+      <c r="C82" s="114">
         <v>-2</v>
       </c>
-      <c r="D82" s="80">
-        <v>0</v>
-      </c>
-      <c r="E82" s="81" t="s">
+      <c r="D82" s="121">
+        <v>0</v>
+      </c>
+      <c r="E82" s="122" t="s">
         <v>185</v>
       </c>
-      <c r="F82" s="122"/>
+      <c r="F82" s="74"/>
       <c r="G82" s="36" t="s">
         <v>0</v>
       </c>
@@ -3462,12 +3474,12 @@
       </c>
     </row>
     <row r="83" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A83" s="87"/>
-      <c r="B83" s="85"/>
-      <c r="C83" s="73"/>
-      <c r="D83" s="75"/>
-      <c r="E83" s="77"/>
-      <c r="F83" s="100"/>
+      <c r="A83" s="103"/>
+      <c r="B83" s="102"/>
+      <c r="C83" s="115"/>
+      <c r="D83" s="117"/>
+      <c r="E83" s="118"/>
+      <c r="F83" s="76"/>
       <c r="G83" s="33" t="s">
         <v>1</v>
       </c>
@@ -3475,26 +3487,26 @@
         <v>136</v>
       </c>
       <c r="I83" s="71" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="84" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A84" s="86" t="s">
+      <c r="A84" s="101" t="s">
         <v>180</v>
       </c>
-      <c r="B84" s="85" t="s">
+      <c r="B84" s="102" t="s">
         <v>133</v>
       </c>
-      <c r="C84" s="73">
+      <c r="C84" s="115">
         <v>-1</v>
       </c>
-      <c r="D84" s="75">
-        <v>0</v>
-      </c>
-      <c r="E84" s="77" t="s">
+      <c r="D84" s="117">
+        <v>0</v>
+      </c>
+      <c r="E84" s="118" t="s">
         <v>185</v>
       </c>
-      <c r="F84" s="98"/>
+      <c r="F84" s="72"/>
       <c r="G84" s="31" t="s">
         <v>0</v>
       </c>
@@ -3504,12 +3516,12 @@
       <c r="I84" s="56"/>
     </row>
     <row r="85" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A85" s="86"/>
-      <c r="B85" s="85"/>
-      <c r="C85" s="73"/>
-      <c r="D85" s="75"/>
-      <c r="E85" s="77"/>
-      <c r="F85" s="100"/>
+      <c r="A85" s="101"/>
+      <c r="B85" s="102"/>
+      <c r="C85" s="115"/>
+      <c r="D85" s="117"/>
+      <c r="E85" s="118"/>
+      <c r="F85" s="76"/>
       <c r="G85" s="33" t="s">
         <v>1</v>
       </c>
@@ -3521,22 +3533,22 @@
       </c>
     </row>
     <row r="86" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A86" s="86" t="s">
+      <c r="A86" s="101" t="s">
         <v>181</v>
       </c>
-      <c r="B86" s="85" t="s">
+      <c r="B86" s="102" t="s">
         <v>134</v>
       </c>
-      <c r="C86" s="73">
+      <c r="C86" s="115">
         <v>-1</v>
       </c>
-      <c r="D86" s="75">
-        <v>0</v>
-      </c>
-      <c r="E86" s="77" t="s">
+      <c r="D86" s="117">
+        <v>0</v>
+      </c>
+      <c r="E86" s="118" t="s">
         <v>185</v>
       </c>
-      <c r="F86" s="98"/>
+      <c r="F86" s="72"/>
       <c r="G86" s="31" t="s">
         <v>0</v>
       </c>
@@ -3546,12 +3558,12 @@
       <c r="I86" s="56"/>
     </row>
     <row r="87" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A87" s="88"/>
-      <c r="B87" s="89"/>
-      <c r="C87" s="74"/>
-      <c r="D87" s="76"/>
-      <c r="E87" s="78"/>
-      <c r="F87" s="121"/>
+      <c r="A87" s="111"/>
+      <c r="B87" s="110"/>
+      <c r="C87" s="116"/>
+      <c r="D87" s="119"/>
+      <c r="E87" s="120"/>
+      <c r="F87" s="73"/>
       <c r="G87" s="42" t="s">
         <v>1</v>
       </c>
@@ -3591,53 +3603,110 @@
     </row>
   </sheetData>
   <mergeCells count="175">
-    <mergeCell ref="F86:F87"/>
-    <mergeCell ref="F74:F76"/>
-    <mergeCell ref="F54:F55"/>
-    <mergeCell ref="F56:F58"/>
-    <mergeCell ref="F61:F62"/>
-    <mergeCell ref="F63:F64"/>
-    <mergeCell ref="F65:F66"/>
-    <mergeCell ref="F67:F69"/>
-    <mergeCell ref="F70:F71"/>
-    <mergeCell ref="F82:F83"/>
-    <mergeCell ref="F84:F85"/>
-    <mergeCell ref="F30:F32"/>
-    <mergeCell ref="F33:F35"/>
-    <mergeCell ref="F36:F37"/>
-    <mergeCell ref="F42:F43"/>
-    <mergeCell ref="F44:F45"/>
-    <mergeCell ref="F46:F47"/>
-    <mergeCell ref="F48:F49"/>
-    <mergeCell ref="F50:F51"/>
-    <mergeCell ref="F52:F53"/>
-    <mergeCell ref="F4:F6"/>
-    <mergeCell ref="F7:F9"/>
-    <mergeCell ref="F10:F11"/>
-    <mergeCell ref="F12:F13"/>
-    <mergeCell ref="F14:F16"/>
-    <mergeCell ref="F19:F20"/>
-    <mergeCell ref="F21:F23"/>
-    <mergeCell ref="F24:F25"/>
-    <mergeCell ref="F26:F27"/>
-    <mergeCell ref="A67:A69"/>
-    <mergeCell ref="B67:B69"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="A42:A43"/>
-    <mergeCell ref="B42:B43"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="A65:A66"/>
-    <mergeCell ref="B65:B66"/>
-    <mergeCell ref="A50:A51"/>
-    <mergeCell ref="B50:B51"/>
-    <mergeCell ref="A56:A58"/>
-    <mergeCell ref="B56:B58"/>
+    <mergeCell ref="J42:J43"/>
+    <mergeCell ref="C86:C87"/>
+    <mergeCell ref="D86:D87"/>
+    <mergeCell ref="E86:E87"/>
+    <mergeCell ref="C74:C76"/>
+    <mergeCell ref="D74:D76"/>
+    <mergeCell ref="E74:E76"/>
+    <mergeCell ref="D82:D83"/>
+    <mergeCell ref="E82:E83"/>
+    <mergeCell ref="C84:C85"/>
+    <mergeCell ref="D84:D85"/>
+    <mergeCell ref="E84:E85"/>
+    <mergeCell ref="C67:C69"/>
+    <mergeCell ref="D67:D69"/>
+    <mergeCell ref="E67:E69"/>
+    <mergeCell ref="C70:C71"/>
+    <mergeCell ref="D70:D71"/>
+    <mergeCell ref="E70:E71"/>
+    <mergeCell ref="C63:C64"/>
+    <mergeCell ref="D63:D64"/>
+    <mergeCell ref="E63:E64"/>
+    <mergeCell ref="C65:C66"/>
+    <mergeCell ref="D65:D66"/>
+    <mergeCell ref="E65:E66"/>
+    <mergeCell ref="D56:D58"/>
+    <mergeCell ref="E56:E58"/>
+    <mergeCell ref="C61:C62"/>
+    <mergeCell ref="D61:D62"/>
+    <mergeCell ref="E61:E62"/>
+    <mergeCell ref="C52:C53"/>
+    <mergeCell ref="D52:D53"/>
+    <mergeCell ref="E52:E53"/>
+    <mergeCell ref="C54:C55"/>
+    <mergeCell ref="D54:D55"/>
+    <mergeCell ref="E54:E55"/>
+    <mergeCell ref="D48:D49"/>
+    <mergeCell ref="E48:E49"/>
+    <mergeCell ref="C50:C51"/>
+    <mergeCell ref="D50:D51"/>
+    <mergeCell ref="E50:E51"/>
+    <mergeCell ref="D42:D43"/>
+    <mergeCell ref="E42:E43"/>
+    <mergeCell ref="C44:C45"/>
+    <mergeCell ref="D44:D45"/>
+    <mergeCell ref="E44:E45"/>
+    <mergeCell ref="C46:C47"/>
+    <mergeCell ref="D46:D47"/>
+    <mergeCell ref="E46:E47"/>
+    <mergeCell ref="D30:D32"/>
+    <mergeCell ref="E30:E32"/>
+    <mergeCell ref="C33:C35"/>
+    <mergeCell ref="D33:D35"/>
+    <mergeCell ref="E33:E35"/>
+    <mergeCell ref="C36:C37"/>
+    <mergeCell ref="D36:D37"/>
+    <mergeCell ref="E36:E37"/>
+    <mergeCell ref="D21:D23"/>
+    <mergeCell ref="E21:E23"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="E24:E25"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="D26:D27"/>
+    <mergeCell ref="E26:E27"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="C14:C16"/>
+    <mergeCell ref="D14:D16"/>
+    <mergeCell ref="E14:E16"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="D4:D6"/>
+    <mergeCell ref="E4:E6"/>
+    <mergeCell ref="C7:C9"/>
+    <mergeCell ref="D7:D9"/>
+    <mergeCell ref="E7:E9"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="A74:A76"/>
+    <mergeCell ref="B74:B76"/>
+    <mergeCell ref="C82:C83"/>
+    <mergeCell ref="C4:C6"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="C21:C23"/>
+    <mergeCell ref="C30:C32"/>
+    <mergeCell ref="C42:C43"/>
+    <mergeCell ref="A52:A53"/>
+    <mergeCell ref="B52:B53"/>
+    <mergeCell ref="A54:A55"/>
+    <mergeCell ref="B54:B55"/>
+    <mergeCell ref="A44:A45"/>
+    <mergeCell ref="B44:B45"/>
+    <mergeCell ref="A46:A47"/>
+    <mergeCell ref="B46:B47"/>
+    <mergeCell ref="A48:A49"/>
+    <mergeCell ref="B48:B49"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="A36:A37"/>
+    <mergeCell ref="B36:B37"/>
+    <mergeCell ref="C48:C49"/>
+    <mergeCell ref="C56:C58"/>
     <mergeCell ref="B4:B6"/>
     <mergeCell ref="A4:A6"/>
     <mergeCell ref="A7:A9"/>
@@ -3662,110 +3731,53 @@
     <mergeCell ref="B61:B62"/>
     <mergeCell ref="A63:A64"/>
     <mergeCell ref="B63:B64"/>
-    <mergeCell ref="A74:A76"/>
-    <mergeCell ref="B74:B76"/>
-    <mergeCell ref="C82:C83"/>
-    <mergeCell ref="C4:C6"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="C21:C23"/>
-    <mergeCell ref="C30:C32"/>
-    <mergeCell ref="C42:C43"/>
-    <mergeCell ref="A52:A53"/>
-    <mergeCell ref="B52:B53"/>
-    <mergeCell ref="A54:A55"/>
-    <mergeCell ref="B54:B55"/>
-    <mergeCell ref="A44:A45"/>
-    <mergeCell ref="B44:B45"/>
-    <mergeCell ref="A46:A47"/>
-    <mergeCell ref="B46:B47"/>
-    <mergeCell ref="A48:A49"/>
-    <mergeCell ref="B48:B49"/>
-    <mergeCell ref="A26:A27"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="A36:A37"/>
-    <mergeCell ref="B36:B37"/>
-    <mergeCell ref="C48:C49"/>
-    <mergeCell ref="C56:C58"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="C14:C16"/>
-    <mergeCell ref="D14:D16"/>
-    <mergeCell ref="E14:E16"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="E19:E20"/>
-    <mergeCell ref="D4:D6"/>
-    <mergeCell ref="E4:E6"/>
-    <mergeCell ref="C7:C9"/>
-    <mergeCell ref="D7:D9"/>
-    <mergeCell ref="E7:E9"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="D30:D32"/>
-    <mergeCell ref="E30:E32"/>
-    <mergeCell ref="C33:C35"/>
-    <mergeCell ref="D33:D35"/>
-    <mergeCell ref="E33:E35"/>
-    <mergeCell ref="C36:C37"/>
-    <mergeCell ref="D36:D37"/>
-    <mergeCell ref="E36:E37"/>
-    <mergeCell ref="D21:D23"/>
-    <mergeCell ref="E21:E23"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="E24:E25"/>
-    <mergeCell ref="C26:C27"/>
-    <mergeCell ref="D26:D27"/>
-    <mergeCell ref="E26:E27"/>
-    <mergeCell ref="D48:D49"/>
-    <mergeCell ref="E48:E49"/>
-    <mergeCell ref="C50:C51"/>
-    <mergeCell ref="D50:D51"/>
-    <mergeCell ref="E50:E51"/>
-    <mergeCell ref="D42:D43"/>
-    <mergeCell ref="E42:E43"/>
-    <mergeCell ref="C44:C45"/>
-    <mergeCell ref="D44:D45"/>
-    <mergeCell ref="E44:E45"/>
-    <mergeCell ref="C46:C47"/>
-    <mergeCell ref="D46:D47"/>
-    <mergeCell ref="E46:E47"/>
-    <mergeCell ref="D56:D58"/>
-    <mergeCell ref="E56:E58"/>
-    <mergeCell ref="C61:C62"/>
-    <mergeCell ref="D61:D62"/>
-    <mergeCell ref="E61:E62"/>
-    <mergeCell ref="C52:C53"/>
-    <mergeCell ref="D52:D53"/>
-    <mergeCell ref="E52:E53"/>
-    <mergeCell ref="C54:C55"/>
-    <mergeCell ref="D54:D55"/>
-    <mergeCell ref="E54:E55"/>
-    <mergeCell ref="J42:J43"/>
-    <mergeCell ref="C86:C87"/>
-    <mergeCell ref="D86:D87"/>
-    <mergeCell ref="E86:E87"/>
-    <mergeCell ref="C74:C76"/>
-    <mergeCell ref="D74:D76"/>
-    <mergeCell ref="E74:E76"/>
-    <mergeCell ref="D82:D83"/>
-    <mergeCell ref="E82:E83"/>
-    <mergeCell ref="C84:C85"/>
-    <mergeCell ref="D84:D85"/>
-    <mergeCell ref="E84:E85"/>
-    <mergeCell ref="C67:C69"/>
-    <mergeCell ref="D67:D69"/>
-    <mergeCell ref="E67:E69"/>
-    <mergeCell ref="C70:C71"/>
-    <mergeCell ref="D70:D71"/>
-    <mergeCell ref="E70:E71"/>
-    <mergeCell ref="C63:C64"/>
-    <mergeCell ref="D63:D64"/>
-    <mergeCell ref="E63:E64"/>
-    <mergeCell ref="C65:C66"/>
-    <mergeCell ref="D65:D66"/>
-    <mergeCell ref="E65:E66"/>
+    <mergeCell ref="A67:A69"/>
+    <mergeCell ref="B67:B69"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="A42:A43"/>
+    <mergeCell ref="B42:B43"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="A65:A66"/>
+    <mergeCell ref="B65:B66"/>
+    <mergeCell ref="A50:A51"/>
+    <mergeCell ref="B50:B51"/>
+    <mergeCell ref="A56:A58"/>
+    <mergeCell ref="B56:B58"/>
+    <mergeCell ref="F4:F6"/>
+    <mergeCell ref="F7:F9"/>
+    <mergeCell ref="F10:F11"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="F14:F16"/>
+    <mergeCell ref="F19:F20"/>
+    <mergeCell ref="F21:F23"/>
+    <mergeCell ref="F24:F25"/>
+    <mergeCell ref="F26:F27"/>
+    <mergeCell ref="F30:F32"/>
+    <mergeCell ref="F33:F35"/>
+    <mergeCell ref="F36:F37"/>
+    <mergeCell ref="F42:F43"/>
+    <mergeCell ref="F44:F45"/>
+    <mergeCell ref="F46:F47"/>
+    <mergeCell ref="F48:F49"/>
+    <mergeCell ref="F50:F51"/>
+    <mergeCell ref="F52:F53"/>
+    <mergeCell ref="F86:F87"/>
+    <mergeCell ref="F74:F76"/>
+    <mergeCell ref="F54:F55"/>
+    <mergeCell ref="F56:F58"/>
+    <mergeCell ref="F61:F62"/>
+    <mergeCell ref="F63:F64"/>
+    <mergeCell ref="F65:F66"/>
+    <mergeCell ref="F67:F69"/>
+    <mergeCell ref="F70:F71"/>
+    <mergeCell ref="F82:F83"/>
+    <mergeCell ref="F84:F85"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
@@ -4422,24 +4434,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100DD38B4BA879657459FE8C7022D55B717" ma:contentTypeVersion="15" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="d5c0f8514766e5ee81dc36ef583fe1d6">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns3="b91bfc96-29e1-4fce-b1c9-d4ca10ce5a83" xmlns:ns4="924d9142-22e9-433f-95fb-5e56abb45a2b" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5fda3cd559eb82edd80343133af36ddc" ns1:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -4679,33 +4673,25 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{23051A02-7089-4210-AA65-89A037B4756D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="b91bfc96-29e1-4fce-b1c9-d4ca10ce5a83"/>
-    <ds:schemaRef ds:uri="924d9142-22e9-433f-95fb-5e56abb45a2b"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8CC5B40C-D9DA-48AF-AAFA-80EF387CF828}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{49F939F1-ED95-4D2C-BE48-5C311B9F9B9B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4723,4 +4709,30 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8CC5B40C-D9DA-48AF-AAFA-80EF387CF828}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{23051A02-7089-4210-AA65-89A037B4756D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="b91bfc96-29e1-4fce-b1c9-d4ca10ce5a83"/>
+    <ds:schemaRef ds:uri="924d9142-22e9-433f-95fb-5e56abb45a2b"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>